<commit_message>
Data updated by GitHub Bot (2020-06-16 20:09) (#136)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -256,7 +256,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -393,12 +393,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -510,6 +519,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2025,7 +2039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2111,7 +2125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
@@ -2135,10 +2149,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B82" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R110" sqref="R110"/>
+      <selection pane="bottomRight" activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7194,57 +7208,59 @@
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A103" s="5">
+      <c r="A103" s="55">
         <v>43996</v>
       </c>
-      <c r="B103" s="28">
+      <c r="B103" s="56">
         <v>1088</v>
       </c>
-      <c r="C103" s="28">
+      <c r="C103" s="56">
         <v>327</v>
       </c>
-      <c r="D103" s="28">
+      <c r="D103" s="56">
         <v>261</v>
       </c>
-      <c r="E103" s="28">
+      <c r="E103" s="56">
         <v>885</v>
       </c>
-      <c r="F103" s="28">
+      <c r="F103" s="56">
         <v>952</v>
       </c>
-      <c r="G103" s="28">
+      <c r="G103" s="56">
         <v>1294</v>
       </c>
-      <c r="H103" s="28">
+      <c r="H103" s="56">
         <v>4010</v>
       </c>
-      <c r="I103" s="28">
+      <c r="I103" s="56">
         <v>341</v>
       </c>
-      <c r="J103" s="28">
+      <c r="J103" s="56">
         <v>2035</v>
       </c>
-      <c r="K103" s="28">
+      <c r="K103" s="56">
         <v>2807</v>
       </c>
-      <c r="L103" s="28">
+      <c r="L103" s="56">
         <v>8</v>
       </c>
-      <c r="M103" s="28">
+      <c r="M103" s="56">
         <v>54</v>
       </c>
-      <c r="N103" s="28">
+      <c r="N103" s="56">
         <v>1687</v>
       </c>
-      <c r="O103" s="28">
+      <c r="O103" s="56">
         <v>6</v>
       </c>
-      <c r="P103" s="32">
+      <c r="P103" s="57">
         <v>15755</v>
       </c>
     </row>
     <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="5"/>
+      <c r="A104" s="5">
+        <v>43997</v>
+      </c>
       <c r="C104" s="28"/>
       <c r="D104" s="28"/>
       <c r="E104" s="28"/>
@@ -7263,6 +7279,9 @@
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A105" s="5">
+        <v>43998</v>
+      </c>
       <c r="C105" s="28"/>
       <c r="D105" s="28"/>
       <c r="E105" s="28"/>
@@ -7276,7 +7295,9 @@
       <c r="M105" s="28"/>
       <c r="N105" s="28"/>
       <c r="O105" s="28"/>
-      <c r="P105" s="28"/>
+      <c r="P105" s="28">
+        <v>18045</v>
+      </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C106" s="28"/>
@@ -8213,11 +8234,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q93"/>
+  <dimension ref="A1:Q94"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E101" sqref="E101"/>
+      <pane ySplit="3" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R101" sqref="R101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13092,6 +13113,59 @@
         <v>18</v>
       </c>
     </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A94" s="30">
+        <v>43998</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K94" s="11">
+        <v>6</v>
+      </c>
+      <c r="L94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P94" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q94" s="13">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -13100,13 +13174,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R85"/>
+  <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P94" sqref="P94"/>
+      <selection pane="bottomRight" activeCell="H107" sqref="H107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17560,6 +17634,59 @@
         <v>578</v>
       </c>
     </row>
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A86" s="51">
+        <v>43998</v>
+      </c>
+      <c r="B86" s="11">
+        <v>5</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E86" s="11">
+        <v>56</v>
+      </c>
+      <c r="F86" s="11">
+        <v>7</v>
+      </c>
+      <c r="G86" s="11">
+        <v>58</v>
+      </c>
+      <c r="H86" s="11">
+        <v>255</v>
+      </c>
+      <c r="I86" s="11">
+        <v>7</v>
+      </c>
+      <c r="J86" s="11">
+        <v>44</v>
+      </c>
+      <c r="K86" s="11">
+        <v>131</v>
+      </c>
+      <c r="L86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N86" s="11">
+        <v>4</v>
+      </c>
+      <c r="O86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q86" s="13">
+        <v>567</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -17568,13 +17695,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R96" sqref="R96"/>
+      <selection pane="bottomRight" activeCell="R91" sqref="R91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22025,12 +22152,65 @@
         <v>292</v>
       </c>
     </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" s="30">
+        <v>43998</v>
+      </c>
+      <c r="B86" s="11">
+        <v>26</v>
+      </c>
+      <c r="C86" s="11">
+        <v>19</v>
+      </c>
+      <c r="D86" s="11">
+        <v>12</v>
+      </c>
+      <c r="E86" s="11">
+        <v>15</v>
+      </c>
+      <c r="F86" s="11">
+        <v>36</v>
+      </c>
+      <c r="G86" s="11">
+        <v>19</v>
+      </c>
+      <c r="H86" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I86" s="11">
+        <v>41</v>
+      </c>
+      <c r="J86" s="11">
+        <v>42</v>
+      </c>
+      <c r="K86" s="11">
+        <v>193</v>
+      </c>
+      <c r="L86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N86" s="11">
+        <v>16</v>
+      </c>
+      <c r="O86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P86" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q86" s="13">
+        <v>419</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -22055,7 +22235,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-15T12:45:35Z</value>
+      <value order="0">2020-06-16T12:36:30Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -22067,16 +22247,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Edited</value>
+      <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41747896</value>
+      <value order="0">vA41774359</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">25.8</value>
+      <value order="0">25.10</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">183</value>
+      <value order="0">185</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -22113,7 +22293,7 @@
 </metadata>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-17 20:09) (#140)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -2039,7 +2039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2125,7 +2125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
@@ -2149,10 +2149,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C107" sqref="C107"/>
+      <selection pane="bottomRight" activeCell="P107" sqref="P107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7300,6 +7300,9 @@
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A106" s="5">
+        <v>43999</v>
+      </c>
       <c r="C106" s="28"/>
       <c r="D106" s="28"/>
       <c r="E106" s="28"/>
@@ -7313,7 +7316,9 @@
       <c r="M106" s="28"/>
       <c r="N106" s="28"/>
       <c r="O106" s="28"/>
-      <c r="P106" s="28"/>
+      <c r="P106" s="28">
+        <v>18066</v>
+      </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C107" s="28"/>
@@ -8234,11 +8239,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q94"/>
+  <dimension ref="A1:Q95"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R101" sqref="R101"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13166,6 +13171,59 @@
         <v>19</v>
       </c>
     </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A95" s="30">
+        <v>43999</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J95" s="14">
+        <v>6</v>
+      </c>
+      <c r="K95" s="11">
+        <v>6</v>
+      </c>
+      <c r="L95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P95" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q95" s="13">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -13174,13 +13232,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R86"/>
+  <dimension ref="A1:R87"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H107" sqref="H107"/>
+      <selection pane="bottomRight" activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17674,8 +17732,8 @@
       <c r="M86" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="N86" s="11">
-        <v>4</v>
+      <c r="N86" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="O86" s="14" t="s">
         <v>29</v>
@@ -17685,6 +17743,59 @@
       </c>
       <c r="Q86" s="13">
         <v>567</v>
+      </c>
+    </row>
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A87" s="51">
+        <v>43999</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E87" s="11">
+        <v>56</v>
+      </c>
+      <c r="F87" s="11">
+        <v>6</v>
+      </c>
+      <c r="G87" s="11">
+        <v>55</v>
+      </c>
+      <c r="H87" s="11">
+        <v>256</v>
+      </c>
+      <c r="I87" s="11">
+        <v>5</v>
+      </c>
+      <c r="J87" s="11">
+        <v>38</v>
+      </c>
+      <c r="K87" s="11">
+        <v>131</v>
+      </c>
+      <c r="L87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q87" s="13">
+        <v>553</v>
       </c>
     </row>
   </sheetData>
@@ -17695,13 +17806,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q86"/>
+  <dimension ref="A1:Q87"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R91" sqref="R91"/>
+      <selection pane="bottomRight" activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22203,6 +22314,59 @@
       </c>
       <c r="Q86" s="13">
         <v>419</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87" s="30">
+        <v>43999</v>
+      </c>
+      <c r="B87" s="11">
+        <v>26</v>
+      </c>
+      <c r="C87" s="11">
+        <v>21</v>
+      </c>
+      <c r="D87" s="11">
+        <v>8</v>
+      </c>
+      <c r="E87" s="11">
+        <v>14</v>
+      </c>
+      <c r="F87" s="11">
+        <v>38</v>
+      </c>
+      <c r="G87" s="11">
+        <v>24</v>
+      </c>
+      <c r="H87" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I87" s="11">
+        <v>20</v>
+      </c>
+      <c r="J87" s="11">
+        <v>56</v>
+      </c>
+      <c r="K87" s="11">
+        <v>193</v>
+      </c>
+      <c r="L87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N87" s="11">
+        <v>11</v>
+      </c>
+      <c r="O87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P87" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q87" s="13">
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -22235,7 +22399,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-16T12:36:30Z</value>
+      <value order="0">2020-06-17T12:13:29Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -22250,13 +22414,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41774359</value>
+      <value order="0">vA41801529</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">25.10</value>
+      <value order="0">25.13</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">185</value>
+      <value order="0">188</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-18 20:09) (#145)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1961" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -554,8 +554,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -565,7 +565,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="6962775" cy="14077950"/>
+          <a:ext cx="6962775" cy="14773274"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -757,7 +757,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>he daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory. From 15 June the figures will also include people tested through the UK Government's testing programme including drive through, mobile testing units and home tests. There will be a delay to publishing these but a board table is expected to be available on or before 18 June.</a:t>
+            <a:t>he daily total of people found positive on 2/6/20 contains 40 historic samples from an NHS Fife laboratory. From 15 June the figures  also include people tested through the UK Government's testing programme including drive through, mobile testing units and home tests. The increase on 15 June is due to the addition of all the UKG data on that day.</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB">
             <a:effectLst/>
@@ -799,7 +799,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>3. Where labs do not provide their overnight data in time for the daily publication, the testing figures will then be added to the return for the subsequent day.   </a:t>
+            <a:t>3. Where labs do not provide their overnight data in time for the daily publication, the figures will then be added to the return for the subsequent day.   </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1698,8 +1698,8 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>771072</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>149226</xdr:colOff>
       <xdr:row>102</xdr:row>
       <xdr:rowOff>163284</xdr:rowOff>
     </xdr:from>
@@ -1711,7 +1711,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12709072" y="19122570"/>
+          <a:off x="12406994" y="20267838"/>
           <a:ext cx="5143500" cy="1097643"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1749,10 +1749,20 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>As of 15 June, this includes confirmed cases at UK Government Regional Testing Centres (RTCs). </a:t>
+            <a:t>As of 15 June, includes people</a:t>
           </a:r>
-        </a:p>
-        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> tested</a:t>
+          </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100">
               <a:solidFill>
@@ -1763,9 +1773,57 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>A breakdown by NHS Board is not yet available from UK Gov RTCs for 15 June. This table will be updated by 18 June.</a:t>
+            <a:t> through the UK Government (UKG) testing programme</a:t>
           </a:r>
-          <a:endParaRPr lang="en-GB" sz="1100"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> (Regional Testing Centres, Mobile Testing Units and home testing kits). Prior to 15 June the figures show people tested through NHS labs only. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The increase on 15 June is due to the addition of all the UKG cases to the database. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>For more information see notes .</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB">
+            <a:effectLst/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2039,7 +2097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2125,7 +2183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
@@ -2149,10 +2207,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="I83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P107" sqref="P107"/>
+      <selection pane="bottomRight" activeCell="N119" sqref="N119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7261,20 +7319,49 @@
       <c r="A104" s="5">
         <v>43997</v>
       </c>
-      <c r="C104" s="28"/>
-      <c r="D104" s="28"/>
-      <c r="E104" s="28"/>
-      <c r="F104" s="28"/>
-      <c r="G104" s="28"/>
-      <c r="H104" s="28"/>
-      <c r="I104" s="28"/>
-      <c r="J104" s="28"/>
-      <c r="K104" s="28"/>
-      <c r="L104" s="28"/>
-      <c r="M104" s="28"/>
-      <c r="N104" s="28"/>
-      <c r="O104" s="28"/>
-      <c r="P104" s="32">
+      <c r="B104" s="28">
+        <v>1243</v>
+      </c>
+      <c r="C104" s="28">
+        <v>345</v>
+      </c>
+      <c r="D104" s="28">
+        <v>274</v>
+      </c>
+      <c r="E104" s="28">
+        <v>926</v>
+      </c>
+      <c r="F104" s="28">
+        <v>1048</v>
+      </c>
+      <c r="G104" s="28">
+        <v>1405</v>
+      </c>
+      <c r="H104" s="28">
+        <v>4805</v>
+      </c>
+      <c r="I104" s="28">
+        <v>373</v>
+      </c>
+      <c r="J104" s="28">
+        <v>2671</v>
+      </c>
+      <c r="K104" s="28">
+        <v>3110</v>
+      </c>
+      <c r="L104" s="28">
+        <v>9</v>
+      </c>
+      <c r="M104" s="28">
+        <v>54</v>
+      </c>
+      <c r="N104" s="28">
+        <v>1760</v>
+      </c>
+      <c r="O104" s="28">
+        <v>7</v>
+      </c>
+      <c r="P104" s="34">
         <v>18030</v>
       </c>
     </row>
@@ -7282,20 +7369,49 @@
       <c r="A105" s="5">
         <v>43998</v>
       </c>
-      <c r="C105" s="28"/>
-      <c r="D105" s="28"/>
-      <c r="E105" s="28"/>
-      <c r="F105" s="28"/>
-      <c r="G105" s="28"/>
-      <c r="H105" s="28"/>
-      <c r="I105" s="28"/>
-      <c r="J105" s="28"/>
-      <c r="K105" s="28"/>
-      <c r="L105" s="28"/>
-      <c r="M105" s="28"/>
-      <c r="N105" s="28"/>
-      <c r="O105" s="28"/>
-      <c r="P105" s="28">
+      <c r="B105" s="28">
+        <v>1243</v>
+      </c>
+      <c r="C105" s="28">
+        <v>345</v>
+      </c>
+      <c r="D105" s="28">
+        <v>274</v>
+      </c>
+      <c r="E105" s="28">
+        <v>926</v>
+      </c>
+      <c r="F105" s="28">
+        <v>1051</v>
+      </c>
+      <c r="G105" s="28">
+        <v>1405</v>
+      </c>
+      <c r="H105" s="28">
+        <v>4808</v>
+      </c>
+      <c r="I105" s="28">
+        <v>373</v>
+      </c>
+      <c r="J105" s="28">
+        <v>2674</v>
+      </c>
+      <c r="K105" s="28">
+        <v>3116</v>
+      </c>
+      <c r="L105" s="28">
+        <v>9</v>
+      </c>
+      <c r="M105" s="28">
+        <v>54</v>
+      </c>
+      <c r="N105" s="28">
+        <v>1760</v>
+      </c>
+      <c r="O105" s="28">
+        <v>7</v>
+      </c>
+      <c r="P105" s="32">
         <v>18045</v>
       </c>
     </row>
@@ -7303,38 +7419,101 @@
       <c r="A106" s="5">
         <v>43999</v>
       </c>
-      <c r="C106" s="28"/>
-      <c r="D106" s="28"/>
-      <c r="E106" s="28"/>
-      <c r="F106" s="28"/>
-      <c r="G106" s="28"/>
-      <c r="H106" s="28"/>
-      <c r="I106" s="28"/>
-      <c r="J106" s="28"/>
-      <c r="K106" s="28"/>
-      <c r="L106" s="28"/>
-      <c r="M106" s="28"/>
-      <c r="N106" s="28"/>
-      <c r="O106" s="28"/>
-      <c r="P106" s="28">
+      <c r="B106" s="28">
+        <v>1245</v>
+      </c>
+      <c r="C106" s="28">
+        <v>345</v>
+      </c>
+      <c r="D106" s="28">
+        <v>274</v>
+      </c>
+      <c r="E106" s="28">
+        <v>928</v>
+      </c>
+      <c r="F106" s="28">
+        <v>1051</v>
+      </c>
+      <c r="G106" s="28">
+        <v>1409</v>
+      </c>
+      <c r="H106" s="28">
+        <v>4810</v>
+      </c>
+      <c r="I106" s="28">
+        <v>373</v>
+      </c>
+      <c r="J106" s="28">
+        <v>2678</v>
+      </c>
+      <c r="K106" s="28">
+        <v>3123</v>
+      </c>
+      <c r="L106" s="28">
+        <v>9</v>
+      </c>
+      <c r="M106" s="28">
+        <v>54</v>
+      </c>
+      <c r="N106" s="28">
+        <v>1760</v>
+      </c>
+      <c r="O106" s="28">
+        <v>7</v>
+      </c>
+      <c r="P106" s="32">
         <v>18066</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C107" s="28"/>
-      <c r="D107" s="28"/>
-      <c r="E107" s="28"/>
-      <c r="F107" s="28"/>
-      <c r="G107" s="28"/>
-      <c r="H107" s="28"/>
-      <c r="I107" s="28"/>
-      <c r="J107" s="28"/>
-      <c r="K107" s="28"/>
-      <c r="L107" s="28"/>
-      <c r="M107" s="28"/>
-      <c r="N107" s="28"/>
-      <c r="O107" s="28"/>
-      <c r="P107" s="28"/>
+      <c r="A107" s="5">
+        <v>44000</v>
+      </c>
+      <c r="B107" s="28">
+        <v>1245</v>
+      </c>
+      <c r="C107" s="28">
+        <v>345</v>
+      </c>
+      <c r="D107" s="28">
+        <v>274</v>
+      </c>
+      <c r="E107" s="28">
+        <v>928</v>
+      </c>
+      <c r="F107" s="28">
+        <v>1053</v>
+      </c>
+      <c r="G107" s="28">
+        <v>1410</v>
+      </c>
+      <c r="H107" s="28">
+        <v>4813</v>
+      </c>
+      <c r="I107" s="28">
+        <v>373</v>
+      </c>
+      <c r="J107" s="28">
+        <v>2681</v>
+      </c>
+      <c r="K107" s="28">
+        <v>3125</v>
+      </c>
+      <c r="L107" s="28">
+        <v>9</v>
+      </c>
+      <c r="M107" s="28">
+        <v>54</v>
+      </c>
+      <c r="N107" s="28">
+        <v>1760</v>
+      </c>
+      <c r="O107" s="28">
+        <v>7</v>
+      </c>
+      <c r="P107" s="32">
+        <v>18077</v>
+      </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C108" s="28"/>
@@ -8239,11 +8418,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q95"/>
+  <dimension ref="A1:Q96"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
+      <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13224,6 +13403,59 @@
         <v>24</v>
       </c>
     </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A96" s="30">
+        <v>44000</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J96" s="11">
+        <v>5</v>
+      </c>
+      <c r="K96" s="11">
+        <v>6</v>
+      </c>
+      <c r="L96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O96" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P96" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q96" s="13">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -13232,13 +13464,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R87"/>
+  <dimension ref="A1:R88"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A88" sqref="A88"/>
+      <selection pane="bottomRight" activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17798,6 +18030,59 @@
         <v>553</v>
       </c>
     </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A88" s="51">
+        <v>44000</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E88" s="11">
+        <v>57</v>
+      </c>
+      <c r="F88" s="11">
+        <v>7</v>
+      </c>
+      <c r="G88" s="11">
+        <v>50</v>
+      </c>
+      <c r="H88" s="11">
+        <v>249</v>
+      </c>
+      <c r="I88" s="11">
+        <v>5</v>
+      </c>
+      <c r="J88" s="11">
+        <v>43</v>
+      </c>
+      <c r="K88" s="11">
+        <v>131</v>
+      </c>
+      <c r="L88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q88" s="13">
+        <v>547</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -17806,13 +18091,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q87"/>
+  <dimension ref="A1:Q88"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B54" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A88" sqref="A88"/>
+      <selection pane="bottomRight" activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22367,6 +22652,59 @@
       </c>
       <c r="Q87" s="13">
         <v>412</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A88" s="30">
+        <v>44000</v>
+      </c>
+      <c r="B88" s="11">
+        <v>18</v>
+      </c>
+      <c r="C88" s="11">
+        <v>19</v>
+      </c>
+      <c r="D88" s="11">
+        <v>11</v>
+      </c>
+      <c r="E88" s="11">
+        <v>11</v>
+      </c>
+      <c r="F88" s="11">
+        <v>26</v>
+      </c>
+      <c r="G88" s="11">
+        <v>13</v>
+      </c>
+      <c r="H88" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I88" s="11">
+        <v>23</v>
+      </c>
+      <c r="J88" s="11">
+        <v>50</v>
+      </c>
+      <c r="K88" s="11">
+        <v>193</v>
+      </c>
+      <c r="L88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N88" s="11">
+        <v>14</v>
+      </c>
+      <c r="O88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P88" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q88" s="13">
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -22399,7 +22737,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-17T12:13:29Z</value>
+      <value order="0">2020-06-18T12:46:48Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -22414,13 +22752,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41801529</value>
+      <value order="0">vA41828407</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">25.13</value>
+      <value order="0">25.17</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">188</value>
+      <value order="0">192</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Add PH data source
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U446281\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA19028\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1961" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -2183,7 +2183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O52" sqref="O52"/>
     </sheetView>
   </sheetViews>
@@ -2206,11 +2206,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="I83" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="N119" sqref="N119"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7516,20 +7516,54 @@
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C108" s="28"/>
-      <c r="D108" s="28"/>
-      <c r="E108" s="28"/>
-      <c r="F108" s="28"/>
-      <c r="G108" s="28"/>
-      <c r="H108" s="28"/>
-      <c r="I108" s="28"/>
-      <c r="J108" s="28"/>
-      <c r="K108" s="28"/>
-      <c r="L108" s="28"/>
-      <c r="M108" s="28"/>
-      <c r="N108" s="28"/>
-      <c r="O108" s="28"/>
-      <c r="P108" s="28"/>
+      <c r="A108" s="5">
+        <v>44001</v>
+      </c>
+      <c r="B108" s="28">
+        <v>1248</v>
+      </c>
+      <c r="C108" s="28">
+        <v>345</v>
+      </c>
+      <c r="D108" s="28">
+        <v>284</v>
+      </c>
+      <c r="E108" s="28">
+        <v>928</v>
+      </c>
+      <c r="F108" s="28">
+        <v>1053</v>
+      </c>
+      <c r="G108" s="28">
+        <v>1410</v>
+      </c>
+      <c r="H108" s="28">
+        <v>4814</v>
+      </c>
+      <c r="I108" s="28">
+        <v>373</v>
+      </c>
+      <c r="J108" s="28">
+        <v>2685</v>
+      </c>
+      <c r="K108" s="28">
+        <v>3134</v>
+      </c>
+      <c r="L108" s="28">
+        <v>9</v>
+      </c>
+      <c r="M108" s="28">
+        <v>54</v>
+      </c>
+      <c r="N108" s="28">
+        <v>1760</v>
+      </c>
+      <c r="O108" s="28">
+        <v>7</v>
+      </c>
+      <c r="P108" s="32">
+        <v>18104</v>
+      </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C109" s="28"/>
@@ -7548,6 +7582,7 @@
       <c r="P109" s="28"/>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B110" s="28"/>
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
       <c r="E110" s="28"/>
@@ -7564,6 +7599,7 @@
       <c r="P110" s="28"/>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B111" s="28"/>
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
       <c r="E111" s="28"/>
@@ -7580,6 +7616,7 @@
       <c r="P111" s="28"/>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B112" s="28"/>
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
       <c r="E112" s="28"/>
@@ -7596,6 +7633,7 @@
       <c r="P112" s="28"/>
     </row>
     <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B113" s="28"/>
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
       <c r="E113" s="28"/>
@@ -7612,6 +7650,7 @@
       <c r="P113" s="28"/>
     </row>
     <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B114" s="28"/>
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
       <c r="E114" s="28"/>
@@ -8418,11 +8457,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q96"/>
+  <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A97" sqref="A97"/>
+    <sheetView topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13456,6 +13495,59 @@
         <v>23</v>
       </c>
     </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A97" s="30">
+        <v>44001</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K97" s="11">
+        <v>6</v>
+      </c>
+      <c r="L97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O97" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P97" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q97" s="13">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -13464,13 +13556,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R88"/>
+  <dimension ref="A1:R89"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E83" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A89" sqref="A89"/>
+      <selection pane="bottomRight" activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18083,6 +18175,59 @@
         <v>547</v>
       </c>
     </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A89" s="51">
+        <v>44001</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E89" s="11">
+        <v>53</v>
+      </c>
+      <c r="F89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G89" s="11">
+        <v>48</v>
+      </c>
+      <c r="H89" s="11">
+        <v>241</v>
+      </c>
+      <c r="I89" s="11">
+        <v>6</v>
+      </c>
+      <c r="J89" s="11">
+        <v>39</v>
+      </c>
+      <c r="K89" s="11">
+        <v>131</v>
+      </c>
+      <c r="L89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q89" s="13">
+        <v>528</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -18091,13 +18236,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q88"/>
+  <dimension ref="A1:Q89"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A89" sqref="A89"/>
+      <selection pane="bottomRight" activeCell="A90" sqref="A90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22707,12 +22852,65 @@
         <v>382</v>
       </c>
     </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A89" s="30">
+        <v>44001</v>
+      </c>
+      <c r="B89" s="11">
+        <v>20</v>
+      </c>
+      <c r="C89" s="11">
+        <v>20</v>
+      </c>
+      <c r="D89" s="11">
+        <v>12</v>
+      </c>
+      <c r="E89" s="11">
+        <v>18</v>
+      </c>
+      <c r="F89" s="11">
+        <v>33</v>
+      </c>
+      <c r="G89" s="11">
+        <v>13</v>
+      </c>
+      <c r="H89" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I89" s="11">
+        <v>21</v>
+      </c>
+      <c r="J89" s="11">
+        <v>30</v>
+      </c>
+      <c r="K89" s="11">
+        <v>193</v>
+      </c>
+      <c r="L89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N89" s="11">
+        <v>15</v>
+      </c>
+      <c r="O89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P89" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q89" s="13">
+        <v>376</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=customXML/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -22731,13 +22929,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">false</value>
+      <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0"/>
+      <value order="0">2020-06-19T12:49:38Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-18T12:46:48Z</value>
+      <value order="0">2020-06-19T12:49:38Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -22749,16 +22947,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Drafted</value>
+      <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41828407</value>
+      <value order="0">vA41853927</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">25.17</value>
+      <value order="0">26.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">192</value>
+      <value order="0">196</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -22795,7 +22993,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXML/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-20 20:08) (#153)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U446281\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA19028\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\scotland.gov.uk\dc2\fs3_home\u205774\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6050" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2016" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1669,6 +1669,64 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>11. As</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> at 20/06/20, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Lothian data on confirmed</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> and suspected covid-19 hosptial inpatients is under investigation from 16/06/2020 onwards.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" b="0">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-GB" sz="1100">
             <a:effectLst/>
             <a:latin typeface="+mn-lt"/>
@@ -1824,6 +1882,160 @@
           <a:endParaRPr lang="en-GB">
             <a:effectLst/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>547688</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>154782</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3845718" cy="333374"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12811126" y="16644938"/>
+          <a:ext cx="3845718" cy="333374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>* Lothian data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> from 16/06/2020 onwards under investigation.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3845718" cy="357188"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12644438" y="16680656"/>
+          <a:ext cx="3845718" cy="357188"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>* Lothian data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> from 16/06/2020 onwards under investigation.</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2097,23 +2309,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.42578125" style="2"/>
+    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.453125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -2121,7 +2333,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -2129,13 +2341,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -2143,7 +2355,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -2151,7 +2363,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -2159,7 +2371,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -2183,16 +2395,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O52" sqref="O52"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="V71" sqref="V71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.42578125" style="2"/>
+    <col min="1" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="43"/>
     </row>
   </sheetData>
@@ -2206,21 +2418,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B85" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="G94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5703125" style="2"/>
+    <col min="2" max="16" width="11.453125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2240,7 +2452,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -2259,7 +2471,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2309,7 +2521,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -2359,7 +2571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -2409,7 +2621,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -2459,7 +2671,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -2509,7 +2721,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -2559,7 +2771,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -2609,7 +2821,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -2659,7 +2871,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -2709,7 +2921,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -2759,7 +2971,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -2809,7 +3021,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -2859,7 +3071,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -2909,7 +3121,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -2959,7 +3171,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -3009,7 +3221,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -3059,7 +3271,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -3109,7 +3321,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -3159,7 +3371,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -3209,7 +3421,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -3259,7 +3471,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -3309,7 +3521,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -3359,7 +3571,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -3409,7 +3621,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -3459,7 +3671,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -3509,7 +3721,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -3559,7 +3771,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -3609,7 +3821,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -3659,7 +3871,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -3709,7 +3921,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -3759,7 +3971,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -3809,7 +4021,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -3859,7 +4071,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -3909,7 +4121,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -3959,7 +4171,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -4009,7 +4221,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -4059,7 +4271,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -4109,7 +4321,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -4159,7 +4371,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -4209,7 +4421,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -4259,7 +4471,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -4309,7 +4521,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -4359,7 +4571,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -4409,7 +4621,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -4459,7 +4671,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -4509,7 +4721,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -4559,7 +4771,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -4609,7 +4821,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -4659,7 +4871,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -4709,7 +4921,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -4759,7 +4971,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -4809,7 +5021,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -4860,7 +5072,7 @@
       </c>
       <c r="R54" s="38"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -4911,7 +5123,7 @@
       </c>
       <c r="R55" s="38"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -4962,7 +5174,7 @@
       </c>
       <c r="R56" s="39"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -5012,7 +5224,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -5063,7 +5275,7 @@
       </c>
       <c r="R58" s="38"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -5115,7 +5327,7 @@
       <c r="R59" s="38"/>
       <c r="S59" s="38"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -5165,7 +5377,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -5215,7 +5427,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -5265,7 +5477,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -5315,7 +5527,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -5365,7 +5577,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -5415,7 +5627,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -5465,7 +5677,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -5515,7 +5727,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -5565,7 +5777,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -5615,7 +5827,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -5665,7 +5877,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -5715,7 +5927,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -5765,7 +5977,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -5815,7 +6027,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -5865,7 +6077,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -5915,7 +6127,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -5965,7 +6177,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -6015,7 +6227,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -6065,7 +6277,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -6115,7 +6327,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -6165,7 +6377,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -6215,7 +6427,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -6265,7 +6477,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -6315,7 +6527,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -6365,7 +6577,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -6415,7 +6627,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -6465,7 +6677,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -6515,7 +6727,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -6565,7 +6777,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -6615,7 +6827,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -6665,7 +6877,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -6715,7 +6927,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -6765,7 +6977,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -6815,7 +7027,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -6865,7 +7077,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -6915,7 +7127,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -6965,7 +7177,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -7015,7 +7227,7 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>43991</v>
       </c>
@@ -7065,7 +7277,7 @@
         <v>15653</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>43992</v>
       </c>
@@ -7115,7 +7327,7 @@
         <v>15665</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>43993</v>
       </c>
@@ -7165,7 +7377,7 @@
         <v>15682</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>43994</v>
       </c>
@@ -7215,7 +7427,7 @@
         <v>15709</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>43995</v>
       </c>
@@ -7265,7 +7477,7 @@
         <v>15730</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103" s="55">
         <v>43996</v>
       </c>
@@ -7315,7 +7527,7 @@
         <v>15755</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>43997</v>
       </c>
@@ -7365,7 +7577,7 @@
         <v>18030</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>43998</v>
       </c>
@@ -7415,7 +7627,7 @@
         <v>18045</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>43999</v>
       </c>
@@ -7465,7 +7677,7 @@
         <v>18066</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>44000</v>
       </c>
@@ -7515,7 +7727,7 @@
         <v>18077</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>44001</v>
       </c>
@@ -7565,23 +7777,57 @@
         <v>18104</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C109" s="28"/>
-      <c r="D109" s="28"/>
-      <c r="E109" s="28"/>
-      <c r="F109" s="28"/>
-      <c r="G109" s="28"/>
-      <c r="H109" s="28"/>
-      <c r="I109" s="28"/>
-      <c r="J109" s="28"/>
-      <c r="K109" s="28"/>
-      <c r="L109" s="28"/>
-      <c r="M109" s="28"/>
-      <c r="N109" s="28"/>
-      <c r="O109" s="28"/>
-      <c r="P109" s="28"/>
-    </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A109" s="5">
+        <v>44002</v>
+      </c>
+      <c r="B109" s="28">
+        <v>1249</v>
+      </c>
+      <c r="C109" s="28">
+        <v>345</v>
+      </c>
+      <c r="D109" s="28">
+        <v>284</v>
+      </c>
+      <c r="E109" s="28">
+        <v>928</v>
+      </c>
+      <c r="F109" s="28">
+        <v>1055</v>
+      </c>
+      <c r="G109" s="28">
+        <v>1410</v>
+      </c>
+      <c r="H109" s="28">
+        <v>4819</v>
+      </c>
+      <c r="I109" s="28">
+        <v>373</v>
+      </c>
+      <c r="J109" s="28">
+        <v>2698</v>
+      </c>
+      <c r="K109" s="28">
+        <v>3139</v>
+      </c>
+      <c r="L109" s="28">
+        <v>9</v>
+      </c>
+      <c r="M109" s="28">
+        <v>54</v>
+      </c>
+      <c r="N109" s="28">
+        <v>1760</v>
+      </c>
+      <c r="O109" s="28">
+        <v>7</v>
+      </c>
+      <c r="P109" s="32">
+        <v>18130</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B110" s="28"/>
       <c r="C110" s="28"/>
       <c r="D110" s="28"/>
@@ -7598,7 +7844,7 @@
       <c r="O110" s="28"/>
       <c r="P110" s="28"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B111" s="28"/>
       <c r="C111" s="28"/>
       <c r="D111" s="28"/>
@@ -7615,7 +7861,7 @@
       <c r="O111" s="28"/>
       <c r="P111" s="28"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B112" s="28"/>
       <c r="C112" s="28"/>
       <c r="D112" s="28"/>
@@ -7632,7 +7878,7 @@
       <c r="O112" s="28"/>
       <c r="P112" s="28"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B113" s="28"/>
       <c r="C113" s="28"/>
       <c r="D113" s="28"/>
@@ -7649,7 +7895,7 @@
       <c r="O113" s="28"/>
       <c r="P113" s="28"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B114" s="28"/>
       <c r="C114" s="28"/>
       <c r="D114" s="28"/>
@@ -7666,7 +7912,7 @@
       <c r="O114" s="28"/>
       <c r="P114" s="28"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B115" s="28"/>
       <c r="C115" s="28"/>
       <c r="D115" s="28"/>
@@ -7683,7 +7929,7 @@
       <c r="O115" s="28"/>
       <c r="P115" s="28"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B116" s="28"/>
       <c r="C116" s="28"/>
       <c r="D116" s="28"/>
@@ -7700,7 +7946,7 @@
       <c r="O116" s="28"/>
       <c r="P116" s="28"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B117" s="28"/>
       <c r="C117" s="28"/>
       <c r="D117" s="28"/>
@@ -7717,7 +7963,7 @@
       <c r="O117" s="28"/>
       <c r="P117" s="28"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B118" s="28"/>
       <c r="C118" s="28"/>
       <c r="D118" s="28"/>
@@ -7734,7 +7980,7 @@
       <c r="O118" s="28"/>
       <c r="P118" s="28"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B119" s="28"/>
       <c r="C119" s="28"/>
       <c r="D119" s="28"/>
@@ -7751,7 +7997,7 @@
       <c r="O119" s="28"/>
       <c r="P119" s="28"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B120" s="28"/>
       <c r="C120" s="28"/>
       <c r="D120" s="28"/>
@@ -7768,7 +8014,7 @@
       <c r="O120" s="28"/>
       <c r="P120" s="28"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B121" s="28"/>
       <c r="C121" s="28"/>
       <c r="D121" s="28"/>
@@ -7785,7 +8031,7 @@
       <c r="O121" s="28"/>
       <c r="P121" s="28"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B122" s="28"/>
       <c r="C122" s="28"/>
       <c r="D122" s="28"/>
@@ -7802,7 +8048,7 @@
       <c r="O122" s="28"/>
       <c r="P122" s="28"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B123" s="28"/>
       <c r="C123" s="28"/>
       <c r="D123" s="28"/>
@@ -7819,7 +8065,7 @@
       <c r="O123" s="28"/>
       <c r="P123" s="28"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B124" s="28"/>
       <c r="C124" s="28"/>
       <c r="D124" s="28"/>
@@ -7836,7 +8082,7 @@
       <c r="O124" s="28"/>
       <c r="P124" s="28"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B125" s="28"/>
       <c r="C125" s="28"/>
       <c r="D125" s="28"/>
@@ -7853,7 +8099,7 @@
       <c r="O125" s="28"/>
       <c r="P125" s="28"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B126" s="28"/>
       <c r="C126" s="28"/>
       <c r="D126" s="28"/>
@@ -7870,7 +8116,7 @@
       <c r="O126" s="28"/>
       <c r="P126" s="28"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B127" s="28"/>
       <c r="C127" s="28"/>
       <c r="D127" s="28"/>
@@ -7887,7 +8133,7 @@
       <c r="O127" s="28"/>
       <c r="P127" s="28"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B128" s="28"/>
       <c r="C128" s="28"/>
       <c r="D128" s="28"/>
@@ -7904,7 +8150,7 @@
       <c r="O128" s="28"/>
       <c r="P128" s="28"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B129" s="28"/>
       <c r="C129" s="28"/>
       <c r="D129" s="28"/>
@@ -7921,7 +8167,7 @@
       <c r="O129" s="28"/>
       <c r="P129" s="28"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B130" s="28"/>
       <c r="C130" s="28"/>
       <c r="D130" s="28"/>
@@ -7938,7 +8184,7 @@
       <c r="O130" s="28"/>
       <c r="P130" s="28"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B131" s="28"/>
       <c r="C131" s="28"/>
       <c r="D131" s="28"/>
@@ -7955,7 +8201,7 @@
       <c r="O131" s="28"/>
       <c r="P131" s="28"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B132" s="28"/>
       <c r="C132" s="28"/>
       <c r="D132" s="28"/>
@@ -7972,7 +8218,7 @@
       <c r="O132" s="28"/>
       <c r="P132" s="28"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B133" s="28"/>
       <c r="C133" s="28"/>
       <c r="D133" s="28"/>
@@ -7989,7 +8235,7 @@
       <c r="O133" s="28"/>
       <c r="P133" s="28"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B134" s="28"/>
       <c r="C134" s="28"/>
       <c r="D134" s="28"/>
@@ -8006,7 +8252,7 @@
       <c r="O134" s="28"/>
       <c r="P134" s="28"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B135" s="28"/>
       <c r="C135" s="28"/>
       <c r="D135" s="28"/>
@@ -8023,7 +8269,7 @@
       <c r="O135" s="28"/>
       <c r="P135" s="28"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B136" s="28"/>
       <c r="C136" s="28"/>
       <c r="D136" s="28"/>
@@ -8040,7 +8286,7 @@
       <c r="O136" s="28"/>
       <c r="P136" s="28"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B137" s="28"/>
       <c r="C137" s="28"/>
       <c r="D137" s="28"/>
@@ -8057,7 +8303,7 @@
       <c r="O137" s="28"/>
       <c r="P137" s="28"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B138" s="28"/>
       <c r="C138" s="28"/>
       <c r="D138" s="28"/>
@@ -8074,7 +8320,7 @@
       <c r="O138" s="28"/>
       <c r="P138" s="28"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B139" s="28"/>
       <c r="C139" s="28"/>
       <c r="D139" s="28"/>
@@ -8091,7 +8337,7 @@
       <c r="O139" s="28"/>
       <c r="P139" s="28"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B140" s="28"/>
       <c r="C140" s="28"/>
       <c r="D140" s="28"/>
@@ -8108,7 +8354,7 @@
       <c r="O140" s="28"/>
       <c r="P140" s="28"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B141" s="28"/>
       <c r="C141" s="28"/>
       <c r="D141" s="28"/>
@@ -8125,7 +8371,7 @@
       <c r="O141" s="28"/>
       <c r="P141" s="28"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B142" s="28"/>
       <c r="C142" s="28"/>
       <c r="D142" s="28"/>
@@ -8142,7 +8388,7 @@
       <c r="O142" s="28"/>
       <c r="P142" s="28"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B143" s="28"/>
       <c r="C143" s="28"/>
       <c r="D143" s="28"/>
@@ -8159,7 +8405,7 @@
       <c r="O143" s="28"/>
       <c r="P143" s="28"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B144" s="28"/>
       <c r="C144" s="28"/>
       <c r="D144" s="28"/>
@@ -8176,7 +8422,7 @@
       <c r="O144" s="28"/>
       <c r="P144" s="28"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B145" s="28"/>
       <c r="C145" s="28"/>
       <c r="D145" s="28"/>
@@ -8193,7 +8439,7 @@
       <c r="O145" s="28"/>
       <c r="P145" s="28"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B146" s="28"/>
       <c r="C146" s="28"/>
       <c r="D146" s="28"/>
@@ -8210,7 +8456,7 @@
       <c r="O146" s="28"/>
       <c r="P146" s="28"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B147" s="28"/>
       <c r="C147" s="28"/>
       <c r="D147" s="28"/>
@@ -8227,7 +8473,7 @@
       <c r="O147" s="28"/>
       <c r="P147" s="28"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B148" s="28"/>
       <c r="C148" s="28"/>
       <c r="D148" s="28"/>
@@ -8244,7 +8490,7 @@
       <c r="O148" s="28"/>
       <c r="P148" s="28"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B149" s="28"/>
       <c r="C149" s="28"/>
       <c r="D149" s="28"/>
@@ -8261,7 +8507,7 @@
       <c r="O149" s="28"/>
       <c r="P149" s="28"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B150" s="28"/>
       <c r="C150" s="28"/>
       <c r="D150" s="28"/>
@@ -8278,7 +8524,7 @@
       <c r="O150" s="28"/>
       <c r="P150" s="28"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B151" s="28"/>
       <c r="C151" s="28"/>
       <c r="D151" s="28"/>
@@ -8295,7 +8541,7 @@
       <c r="O151" s="28"/>
       <c r="P151" s="28"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B152" s="28"/>
       <c r="C152" s="28"/>
       <c r="D152" s="28"/>
@@ -8312,7 +8558,7 @@
       <c r="O152" s="28"/>
       <c r="P152" s="28"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B153" s="28"/>
       <c r="C153" s="28"/>
       <c r="D153" s="28"/>
@@ -8329,7 +8575,7 @@
       <c r="O153" s="28"/>
       <c r="P153" s="28"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B154" s="28"/>
       <c r="C154" s="28"/>
       <c r="D154" s="28"/>
@@ -8346,7 +8592,7 @@
       <c r="O154" s="28"/>
       <c r="P154" s="28"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B155" s="28"/>
       <c r="C155" s="28"/>
       <c r="D155" s="28"/>
@@ -8363,7 +8609,7 @@
       <c r="O155" s="28"/>
       <c r="P155" s="28"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B156" s="28"/>
       <c r="C156" s="28"/>
       <c r="D156" s="28"/>
@@ -8380,7 +8626,7 @@
       <c r="O156" s="28"/>
       <c r="P156" s="28"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B157" s="28"/>
       <c r="C157" s="28"/>
       <c r="D157" s="28"/>
@@ -8397,7 +8643,7 @@
       <c r="O157" s="28"/>
       <c r="P157" s="28"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B158" s="28"/>
       <c r="C158" s="28"/>
       <c r="D158" s="28"/>
@@ -8414,7 +8660,7 @@
       <c r="O158" s="28"/>
       <c r="P158" s="28"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B159" s="28"/>
       <c r="C159" s="28"/>
       <c r="D159" s="28"/>
@@ -8431,7 +8677,7 @@
       <c r="O159" s="28"/>
       <c r="P159" s="28"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B160" s="28"/>
       <c r="C160" s="28"/>
       <c r="D160" s="28"/>
@@ -8457,21 +8703,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q97"/>
+  <dimension ref="A1:Q98"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A98" sqref="A98"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S93" sqref="S93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -8492,7 +8738,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -8513,7 +8759,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -8566,7 +8812,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -8619,7 +8865,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -8672,7 +8918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -8725,7 +8971,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -8778,7 +9024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -8831,7 +9077,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -8884,7 +9130,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -8937,7 +9183,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -8990,7 +9236,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -9043,7 +9289,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -9096,7 +9342,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -9149,7 +9395,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -9202,7 +9448,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -9255,7 +9501,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -9308,7 +9554,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -9361,7 +9607,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -9414,7 +9660,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -9467,7 +9713,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -9520,7 +9766,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -9573,7 +9819,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -9626,7 +9872,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -9679,7 +9925,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -9732,7 +9978,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -9785,7 +10031,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -9838,7 +10084,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -9891,7 +10137,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -9944,7 +10190,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -9997,7 +10243,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -10050,7 +10296,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -10103,7 +10349,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -10156,7 +10402,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -10209,7 +10455,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -10262,7 +10508,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43940</v>
       </c>
@@ -10315,7 +10561,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43941</v>
       </c>
@@ -10368,7 +10614,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43942</v>
       </c>
@@ -10421,7 +10667,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43943</v>
       </c>
@@ -10474,7 +10720,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43944</v>
       </c>
@@ -10527,7 +10773,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43945</v>
       </c>
@@ -10580,7 +10826,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43946</v>
       </c>
@@ -10633,7 +10879,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43947</v>
       </c>
@@ -10686,7 +10932,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43948</v>
       </c>
@@ -10739,7 +10985,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43949</v>
       </c>
@@ -10792,7 +11038,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43950</v>
       </c>
@@ -10845,7 +11091,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43951</v>
       </c>
@@ -10898,7 +11144,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43952</v>
       </c>
@@ -10951,7 +11197,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43953</v>
       </c>
@@ -11004,7 +11250,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43954</v>
       </c>
@@ -11057,7 +11303,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43955</v>
       </c>
@@ -11110,7 +11356,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43956</v>
       </c>
@@ -11163,7 +11409,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43957</v>
       </c>
@@ -11216,7 +11462,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43958</v>
       </c>
@@ -11269,7 +11515,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43959</v>
       </c>
@@ -11322,7 +11568,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43960</v>
       </c>
@@ -11375,7 +11621,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43961</v>
       </c>
@@ -11428,7 +11674,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43962</v>
       </c>
@@ -11481,7 +11727,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43963</v>
       </c>
@@ -11534,7 +11780,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43964</v>
       </c>
@@ -11587,7 +11833,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43965</v>
       </c>
@@ -11640,7 +11886,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43966</v>
       </c>
@@ -11693,7 +11939,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43967</v>
       </c>
@@ -11746,7 +11992,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43968</v>
       </c>
@@ -11799,7 +12045,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="30">
         <v>43969</v>
       </c>
@@ -11852,7 +12098,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>43970</v>
       </c>
@@ -11905,7 +12151,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>43971</v>
       </c>
@@ -11958,7 +12204,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="30">
         <v>43972</v>
       </c>
@@ -12011,7 +12257,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="30">
         <v>43973</v>
       </c>
@@ -12064,7 +12310,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="30">
         <v>43974</v>
       </c>
@@ -12117,7 +12363,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="30">
         <v>43975</v>
       </c>
@@ -12170,7 +12416,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="30">
         <v>43976</v>
       </c>
@@ -12223,7 +12469,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="30">
         <v>43977</v>
       </c>
@@ -12276,7 +12522,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="30">
         <v>43978</v>
       </c>
@@ -12329,7 +12575,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="30">
         <v>43979</v>
       </c>
@@ -12382,7 +12628,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="30">
         <v>43980</v>
       </c>
@@ -12435,7 +12681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="30">
         <v>43981</v>
       </c>
@@ -12488,7 +12734,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="30">
         <v>43982</v>
       </c>
@@ -12541,7 +12787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="30">
         <v>43983</v>
       </c>
@@ -12594,7 +12840,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="30">
         <v>43984</v>
       </c>
@@ -12647,7 +12893,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="30">
         <v>43985</v>
       </c>
@@ -12700,7 +12946,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="30">
         <v>43986</v>
       </c>
@@ -12753,7 +12999,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="30">
         <v>43987</v>
       </c>
@@ -12806,7 +13052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="30">
         <v>43988</v>
       </c>
@@ -12859,7 +13105,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" s="30">
         <v>43989</v>
       </c>
@@ -12912,7 +13158,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" s="30">
         <v>43990</v>
       </c>
@@ -12965,7 +13211,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" s="30">
         <v>43991</v>
       </c>
@@ -13018,7 +13264,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88" s="30">
         <v>43992</v>
       </c>
@@ -13071,7 +13317,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89" s="30">
         <v>43993</v>
       </c>
@@ -13124,7 +13370,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A90" s="30">
         <v>43994</v>
       </c>
@@ -13177,7 +13423,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A91" s="30">
         <v>43995</v>
       </c>
@@ -13230,7 +13476,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92" s="30">
         <v>43996</v>
       </c>
@@ -13283,7 +13529,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A93" s="30">
         <v>43997</v>
       </c>
@@ -13336,7 +13582,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A94" s="30">
         <v>43998</v>
       </c>
@@ -13389,7 +13635,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95" s="30">
         <v>43999</v>
       </c>
@@ -13442,7 +13688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96" s="30">
         <v>44000</v>
       </c>
@@ -13495,7 +13741,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A97" s="30">
         <v>44001</v>
       </c>
@@ -13546,6 +13792,59 @@
       </c>
       <c r="Q97" s="13">
         <v>19</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A98" s="30">
+        <v>44002</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K98" s="11">
+        <v>6</v>
+      </c>
+      <c r="L98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O98" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P98" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q98" s="13">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -13556,23 +13855,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R89"/>
+  <dimension ref="A1:R90"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="E83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E61" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A90" sqref="A90"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="15.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -13593,7 +13892,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -13614,7 +13913,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -13667,7 +13966,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -13720,7 +14019,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -13773,7 +14072,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -13826,7 +14125,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -13879,7 +14178,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -13932,7 +14231,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -13985,7 +14284,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -14038,7 +14337,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -14091,7 +14390,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -14144,7 +14443,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -14197,7 +14496,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -14250,7 +14549,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -14303,7 +14602,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -14356,7 +14655,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -14409,7 +14708,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -14462,7 +14761,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -14515,7 +14814,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -14568,7 +14867,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -14621,7 +14920,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -14674,7 +14973,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -14727,7 +15026,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -14780,7 +15079,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -14833,7 +15132,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -14886,7 +15185,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -14939,7 +15238,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -14992,7 +15291,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -15045,7 +15344,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -15098,7 +15397,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -15151,7 +15450,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -15204,7 +15503,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -15257,7 +15556,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -15310,7 +15609,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -15363,7 +15662,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -15416,7 +15715,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -15469,7 +15768,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -15522,7 +15821,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -15575,7 +15874,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -15628,7 +15927,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -15681,7 +15980,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -15734,7 +16033,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -15787,7 +16086,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -15840,7 +16139,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -15893,7 +16192,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -15946,7 +16245,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -15999,7 +16298,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -16052,7 +16351,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -16105,7 +16404,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -16158,7 +16457,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -16211,7 +16510,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -16264,7 +16563,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -16317,7 +16616,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -16370,7 +16669,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -16423,7 +16722,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -16476,7 +16775,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -16529,7 +16828,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -16582,7 +16881,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -16635,7 +16934,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -16688,7 +16987,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -16741,7 +17040,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -16794,7 +17093,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -16847,7 +17146,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -16900,7 +17199,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" s="51">
         <v>43977</v>
       </c>
@@ -16953,7 +17252,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="51">
         <v>43978</v>
       </c>
@@ -17006,7 +17305,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="51">
         <v>43979</v>
       </c>
@@ -17059,7 +17358,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="51">
         <v>43980</v>
       </c>
@@ -17112,7 +17411,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="51">
         <v>43981</v>
       </c>
@@ -17165,7 +17464,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="51">
         <v>43982</v>
       </c>
@@ -17218,7 +17517,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="51">
         <v>43983</v>
       </c>
@@ -17271,7 +17570,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" s="51">
         <v>43984</v>
       </c>
@@ -17324,7 +17623,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A73" s="51">
         <v>43985</v>
       </c>
@@ -17377,7 +17676,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" s="51">
         <v>43986</v>
       </c>
@@ -17430,7 +17729,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75" s="51">
         <v>43987</v>
       </c>
@@ -17483,7 +17782,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76" s="51">
         <v>43988</v>
       </c>
@@ -17536,7 +17835,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" s="51">
         <v>43989</v>
       </c>
@@ -17589,7 +17888,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78" s="51">
         <v>43990</v>
       </c>
@@ -17642,7 +17941,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" s="51">
         <v>43991</v>
       </c>
@@ -17695,7 +17994,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80" s="51">
         <v>43992</v>
       </c>
@@ -17749,7 +18048,7 @@
       </c>
       <c r="R80" s="54"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A81" s="51">
         <v>43993</v>
       </c>
@@ -17803,7 +18102,7 @@
       </c>
       <c r="R81" s="54"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A82" s="51">
         <v>43994</v>
       </c>
@@ -17857,7 +18156,7 @@
       </c>
       <c r="R82" s="54"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A83" s="51">
         <v>43995</v>
       </c>
@@ -17910,7 +18209,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A84" s="51">
         <v>43996</v>
       </c>
@@ -17963,7 +18262,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A85" s="51">
         <v>43997</v>
       </c>
@@ -18016,7 +18315,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A86" s="51">
         <v>43998</v>
       </c>
@@ -18069,7 +18368,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A87" s="51">
         <v>43999</v>
       </c>
@@ -18122,7 +18421,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A88" s="51">
         <v>44000</v>
       </c>
@@ -18175,7 +18474,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A89" s="51">
         <v>44001</v>
       </c>
@@ -18226,33 +18525,87 @@
       </c>
       <c r="Q89" s="13">
         <v>528</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A90" s="51">
+        <v>44002</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E90" s="11">
+        <v>52</v>
+      </c>
+      <c r="F90" s="11">
+        <v>5</v>
+      </c>
+      <c r="G90" s="11">
+        <v>46</v>
+      </c>
+      <c r="H90" s="11">
+        <v>234</v>
+      </c>
+      <c r="I90" s="11">
+        <v>7</v>
+      </c>
+      <c r="J90" s="11">
+        <v>39</v>
+      </c>
+      <c r="K90" s="11">
+        <v>131</v>
+      </c>
+      <c r="L90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P90" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q90" s="13">
+        <v>519</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q89"/>
+  <dimension ref="A1:Q90"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A90" sqref="A90"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -18273,7 +18626,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>30</v>
       </c>
@@ -18294,7 +18647,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -18347,7 +18700,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -18400,7 +18753,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -18453,7 +18806,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -18506,7 +18859,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -18559,7 +18912,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -18612,7 +18965,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -18665,7 +19018,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -18718,7 +19071,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -18771,7 +19124,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -18824,7 +19177,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -18877,7 +19230,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -18930,7 +19283,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -18983,7 +19336,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -19036,7 +19389,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -19089,7 +19442,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -19142,7 +19495,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -19195,7 +19548,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -19248,7 +19601,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -19301,7 +19654,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -19354,7 +19707,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -19407,7 +19760,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -19460,7 +19813,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -19513,7 +19866,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -19566,7 +19919,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -19619,7 +19972,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -19672,7 +20025,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -19725,7 +20078,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -19778,7 +20131,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -19831,7 +20184,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -19884,7 +20237,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -19937,7 +20290,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -19990,7 +20343,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -20043,7 +20396,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="30">
         <v>43948</v>
       </c>
@@ -20096,7 +20449,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="30">
         <v>43949</v>
       </c>
@@ -20149,7 +20502,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="30">
         <v>43950</v>
       </c>
@@ -20202,7 +20555,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="30">
         <v>43951</v>
       </c>
@@ -20255,7 +20608,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="30">
         <v>43952</v>
       </c>
@@ -20308,7 +20661,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="30">
         <v>43953</v>
       </c>
@@ -20361,7 +20714,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="30">
         <v>43954</v>
       </c>
@@ -20414,7 +20767,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="30">
         <v>43955</v>
       </c>
@@ -20467,7 +20820,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="30">
         <v>43956</v>
       </c>
@@ -20520,7 +20873,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="30">
         <v>43957</v>
       </c>
@@ -20573,7 +20926,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="30">
         <v>43958</v>
       </c>
@@ -20626,7 +20979,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="30">
         <v>43959</v>
       </c>
@@ -20679,7 +21032,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="30">
         <v>43960</v>
       </c>
@@ -20732,7 +21085,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="30">
         <v>43961</v>
       </c>
@@ -20785,7 +21138,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="30">
         <v>43962</v>
       </c>
@@ -20838,7 +21191,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="30">
         <v>43963</v>
       </c>
@@ -20891,7 +21244,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="30">
         <v>43964</v>
       </c>
@@ -20944,7 +21297,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="30">
         <v>43965</v>
       </c>
@@ -20997,7 +21350,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="30">
         <v>43966</v>
       </c>
@@ -21050,7 +21403,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="30">
         <v>43967</v>
       </c>
@@ -21103,7 +21456,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="30">
         <v>43968</v>
       </c>
@@ -21156,7 +21509,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="30">
         <v>43969</v>
       </c>
@@ -21209,7 +21562,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="30">
         <v>43970</v>
       </c>
@@ -21262,7 +21615,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="30">
         <v>43971</v>
       </c>
@@ -21315,7 +21668,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="30">
         <v>43972</v>
       </c>
@@ -21368,7 +21721,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="30">
         <v>43973</v>
       </c>
@@ -21421,7 +21774,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="30">
         <v>43974</v>
       </c>
@@ -21474,7 +21827,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="30">
         <v>43975</v>
       </c>
@@ -21527,7 +21880,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="30">
         <v>43976</v>
       </c>
@@ -21580,7 +21933,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="30">
         <v>43977</v>
       </c>
@@ -21633,7 +21986,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="30">
         <v>43978</v>
       </c>
@@ -21686,7 +22039,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="30">
         <v>43979</v>
       </c>
@@ -21739,7 +22092,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="30">
         <v>43980</v>
       </c>
@@ -21792,7 +22145,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="30">
         <v>43981</v>
       </c>
@@ -21845,7 +22198,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="30">
         <v>43982</v>
       </c>
@@ -21898,7 +22251,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="30">
         <v>43983</v>
       </c>
@@ -21951,7 +22304,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="30">
         <v>43984</v>
       </c>
@@ -22004,7 +22357,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="30">
         <v>43985</v>
       </c>
@@ -22057,7 +22410,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="30">
         <v>43986</v>
       </c>
@@ -22110,7 +22463,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="30">
         <v>43987</v>
       </c>
@@ -22163,7 +22516,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="30">
         <v>43988</v>
       </c>
@@ -22216,7 +22569,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="30">
         <v>43989</v>
       </c>
@@ -22269,7 +22622,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="30">
         <v>43990</v>
       </c>
@@ -22322,7 +22675,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="30">
         <v>43991</v>
       </c>
@@ -22375,7 +22728,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="30">
         <v>43992</v>
       </c>
@@ -22428,7 +22781,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="30">
         <v>43993</v>
       </c>
@@ -22481,7 +22834,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="30">
         <v>43994</v>
       </c>
@@ -22534,7 +22887,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="30">
         <v>43995</v>
       </c>
@@ -22587,7 +22940,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="30">
         <v>43996</v>
       </c>
@@ -22640,7 +22993,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" s="30">
         <v>43997</v>
       </c>
@@ -22693,7 +23046,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" s="30">
         <v>43998</v>
       </c>
@@ -22746,7 +23099,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" s="30">
         <v>43999</v>
       </c>
@@ -22799,7 +23152,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88" s="30">
         <v>44000</v>
       </c>
@@ -22852,7 +23205,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89" s="30">
         <v>44001</v>
       </c>
@@ -22905,12 +23258,66 @@
         <v>376</v>
       </c>
     </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A90" s="30">
+        <v>44002</v>
+      </c>
+      <c r="B90" s="11">
+        <v>18</v>
+      </c>
+      <c r="C90" s="11">
+        <v>27</v>
+      </c>
+      <c r="D90" s="11">
+        <v>8</v>
+      </c>
+      <c r="E90" s="11">
+        <v>17</v>
+      </c>
+      <c r="F90" s="11">
+        <v>22</v>
+      </c>
+      <c r="G90" s="11">
+        <v>22</v>
+      </c>
+      <c r="H90" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I90" s="11">
+        <v>17</v>
+      </c>
+      <c r="J90" s="11">
+        <v>47</v>
+      </c>
+      <c r="K90" s="11">
+        <v>193</v>
+      </c>
+      <c r="L90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N90" s="11">
+        <v>13</v>
+      </c>
+      <c r="O90" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P90" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q90" s="36">
+        <v>384</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=customXML/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA" version="1.0.0">
   <systemFields>
     <field name="Objective-Id">
@@ -22929,13 +23336,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">true</value>
+      <value order="0">false</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0">2020-06-19T12:49:38Z</value>
+      <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-19T12:49:38Z</value>
+      <value order="0">2020-06-20T11:33:16Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -22947,16 +23354,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Published</value>
+      <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41853927</value>
+      <value order="0">vA41864601</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">26.0</value>
+      <value order="0">27.2</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">196</value>
+      <value order="0">201</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>
@@ -22993,7 +23400,7 @@
 </metadata>
 </file>
 
-<file path=customXML/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5745109E-2DDF-40CB-AC2B-FF9B10C90820}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.objective.com/ecm/document/metadata/53D26341A57B383EE0540010E0463CCA"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-22 20:09) (#162)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u201433\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA1432\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U445783\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA18464\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5988" windowHeight="6048" tabRatio="803" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -1617,16 +1617,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> ICU.</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>  The total figures for Scotland have therefor been revised as follows:</a:t>
+            <a:t> ICU.  The total figures for Scotland have therefor been revised as follows:</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB">
             <a:effectLst/>
@@ -2667,25 +2658,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C5:C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.42578125" style="2"/>
+    <col min="2" max="2" width="29.44140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.44140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -2693,7 +2684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -2701,13 +2692,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -2715,7 +2706,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -2723,7 +2714,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -2731,7 +2722,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -2759,12 +2750,12 @@
       <selection activeCell="O81" sqref="O81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.42578125" style="2"/>
+    <col min="1" max="16384" width="9.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
       <c r="A44" s="42"/>
     </row>
   </sheetData>
@@ -2778,21 +2769,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J108" sqref="J108"/>
+      <selection pane="bottomRight" activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5703125" style="2"/>
+    <col min="2" max="16" width="11.44140625" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2812,7 +2803,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -2831,7 +2822,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2881,7 +2872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -2931,7 +2922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -2981,7 +2972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -3031,7 +3022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -3081,7 +3072,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -3131,7 +3122,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -3181,7 +3172,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -3231,7 +3222,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -3281,7 +3272,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -3331,7 +3322,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -3381,7 +3372,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -3431,7 +3422,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -3481,7 +3472,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -3531,7 +3522,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -3581,7 +3572,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -3631,7 +3622,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -3681,7 +3672,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -3731,7 +3722,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -3781,7 +3772,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -3831,7 +3822,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -3881,7 +3872,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -3931,7 +3922,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -3981,7 +3972,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -4031,7 +4022,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -4081,7 +4072,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -4131,7 +4122,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -4181,7 +4172,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -4231,7 +4222,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -4281,7 +4272,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -4331,7 +4322,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -4381,7 +4372,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -4431,7 +4422,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -4481,7 +4472,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -4531,7 +4522,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -4581,7 +4572,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -4631,7 +4622,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -4681,7 +4672,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -4731,7 +4722,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -4781,7 +4772,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -4831,7 +4822,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -4881,7 +4872,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -4931,7 +4922,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -4981,7 +4972,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -5031,7 +5022,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -5081,7 +5072,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -5131,7 +5122,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -5181,7 +5172,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -5231,7 +5222,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -5281,7 +5272,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -5331,7 +5322,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -5381,7 +5372,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -5432,7 +5423,7 @@
       </c>
       <c r="R54" s="37"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -5483,7 +5474,7 @@
       </c>
       <c r="R55" s="37"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -5534,7 +5525,7 @@
       </c>
       <c r="R56" s="38"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -5584,7 +5575,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -5635,7 +5626,7 @@
       </c>
       <c r="R58" s="37"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -5687,7 +5678,7 @@
       <c r="R59" s="37"/>
       <c r="S59" s="37"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -5737,7 +5728,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -5787,7 +5778,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -5837,7 +5828,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -5887,7 +5878,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -5937,7 +5928,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -5987,7 +5978,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -6037,7 +6028,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -6087,7 +6078,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -6137,7 +6128,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -6187,7 +6178,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -6237,7 +6228,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -6287,7 +6278,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -6337,7 +6328,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -6387,7 +6378,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -6437,7 +6428,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -6487,7 +6478,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -6537,7 +6528,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -6587,7 +6578,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -6637,7 +6628,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -6687,7 +6678,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -6737,7 +6728,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -6787,7 +6778,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -6837,7 +6828,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -6887,7 +6878,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -6937,7 +6928,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -6987,7 +6978,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -7037,7 +7028,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -7087,7 +7078,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -7137,7 +7128,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -7187,7 +7178,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -7237,7 +7228,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -7287,7 +7278,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -7337,7 +7328,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -7387,7 +7378,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -7437,7 +7428,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -7487,7 +7478,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -7537,7 +7528,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -7587,7 +7578,7 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" s="5">
         <v>43991</v>
       </c>
@@ -7637,7 +7628,7 @@
         <v>15653</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" s="5">
         <v>43992</v>
       </c>
@@ -7687,7 +7678,7 @@
         <v>15665</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" s="5">
         <v>43993</v>
       </c>
@@ -7737,7 +7728,7 @@
         <v>15682</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" s="5">
         <v>43994</v>
       </c>
@@ -7787,7 +7778,7 @@
         <v>15709</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" s="5">
         <v>43995</v>
       </c>
@@ -7837,7 +7828,7 @@
         <v>15730</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A103" s="53">
         <v>43996</v>
       </c>
@@ -7887,7 +7878,7 @@
         <v>15755</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="5">
         <v>43997</v>
       </c>
@@ -7937,7 +7928,7 @@
         <v>18030</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105" s="5">
         <v>43998</v>
       </c>
@@ -7987,7 +7978,7 @@
         <v>18045</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106" s="5">
         <v>43999</v>
       </c>
@@ -8037,7 +8028,7 @@
         <v>18066</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107" s="5">
         <v>44000</v>
       </c>
@@ -8087,7 +8078,7 @@
         <v>18077</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108" s="5">
         <v>44001</v>
       </c>
@@ -8137,7 +8128,7 @@
         <v>18104</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109" s="5">
         <v>44002</v>
       </c>
@@ -8187,7 +8178,7 @@
         <v>18130</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A110" s="5">
         <v>44003</v>
       </c>
@@ -8237,24 +8228,57 @@
         <v>18156</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B111" s="27"/>
-      <c r="C111" s="27"/>
-      <c r="D111" s="27"/>
-      <c r="E111" s="27"/>
-      <c r="F111" s="27"/>
-      <c r="G111" s="27"/>
-      <c r="H111" s="27"/>
-      <c r="I111" s="27"/>
-      <c r="J111" s="27"/>
-      <c r="K111" s="27"/>
-      <c r="L111" s="27"/>
-      <c r="M111" s="27"/>
-      <c r="N111" s="27"/>
-      <c r="O111" s="27"/>
-      <c r="P111" s="27"/>
-    </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A111" s="5">
+        <v>44004</v>
+      </c>
+      <c r="B111" s="27">
+        <v>1250</v>
+      </c>
+      <c r="C111" s="27">
+        <v>346</v>
+      </c>
+      <c r="D111" s="27">
+        <v>285</v>
+      </c>
+      <c r="E111" s="27">
+        <v>928</v>
+      </c>
+      <c r="F111" s="27">
+        <v>1057</v>
+      </c>
+      <c r="G111" s="27">
+        <v>1412</v>
+      </c>
+      <c r="H111" s="27">
+        <v>4830</v>
+      </c>
+      <c r="I111" s="27">
+        <v>373</v>
+      </c>
+      <c r="J111" s="27">
+        <v>2712</v>
+      </c>
+      <c r="K111" s="27">
+        <v>3146</v>
+      </c>
+      <c r="L111" s="27">
+        <v>9</v>
+      </c>
+      <c r="M111" s="27">
+        <v>54</v>
+      </c>
+      <c r="N111" s="27">
+        <v>1761</v>
+      </c>
+      <c r="O111" s="27">
+        <v>7</v>
+      </c>
+      <c r="P111" s="31">
+        <v>18170</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B112" s="27"/>
       <c r="C112" s="27"/>
       <c r="D112" s="27"/>
@@ -8271,7 +8295,7 @@
       <c r="O112" s="27"/>
       <c r="P112" s="27"/>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B113" s="27"/>
       <c r="C113" s="27"/>
       <c r="D113" s="27"/>
@@ -8288,7 +8312,7 @@
       <c r="O113" s="27"/>
       <c r="P113" s="27"/>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B114" s="27"/>
       <c r="C114" s="27"/>
       <c r="D114" s="27"/>
@@ -8305,7 +8329,7 @@
       <c r="O114" s="27"/>
       <c r="P114" s="27"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B115" s="27"/>
       <c r="C115" s="27"/>
       <c r="D115" s="27"/>
@@ -8322,7 +8346,7 @@
       <c r="O115" s="27"/>
       <c r="P115" s="27"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B116" s="27"/>
       <c r="C116" s="27"/>
       <c r="D116" s="27"/>
@@ -8339,7 +8363,7 @@
       <c r="O116" s="27"/>
       <c r="P116" s="27"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B117" s="27"/>
       <c r="C117" s="27"/>
       <c r="D117" s="27"/>
@@ -8356,7 +8380,7 @@
       <c r="O117" s="27"/>
       <c r="P117" s="27"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B118" s="27"/>
       <c r="C118" s="27"/>
       <c r="D118" s="27"/>
@@ -8373,7 +8397,7 @@
       <c r="O118" s="27"/>
       <c r="P118" s="27"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B119" s="27"/>
       <c r="C119" s="27"/>
       <c r="D119" s="27"/>
@@ -8390,7 +8414,7 @@
       <c r="O119" s="27"/>
       <c r="P119" s="27"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B120" s="27"/>
       <c r="C120" s="27"/>
       <c r="D120" s="27"/>
@@ -8407,7 +8431,7 @@
       <c r="O120" s="27"/>
       <c r="P120" s="27"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B121" s="27"/>
       <c r="C121" s="27"/>
       <c r="D121" s="27"/>
@@ -8424,7 +8448,7 @@
       <c r="O121" s="27"/>
       <c r="P121" s="27"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B122" s="27"/>
       <c r="C122" s="27"/>
       <c r="D122" s="27"/>
@@ -8441,7 +8465,7 @@
       <c r="O122" s="27"/>
       <c r="P122" s="27"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B123" s="27"/>
       <c r="C123" s="27"/>
       <c r="D123" s="27"/>
@@ -8458,7 +8482,7 @@
       <c r="O123" s="27"/>
       <c r="P123" s="27"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B124" s="27"/>
       <c r="C124" s="27"/>
       <c r="D124" s="27"/>
@@ -8475,7 +8499,7 @@
       <c r="O124" s="27"/>
       <c r="P124" s="27"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B125" s="27"/>
       <c r="C125" s="27"/>
       <c r="D125" s="27"/>
@@ -8492,7 +8516,7 @@
       <c r="O125" s="27"/>
       <c r="P125" s="27"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B126" s="27"/>
       <c r="C126" s="27"/>
       <c r="D126" s="27"/>
@@ -8509,7 +8533,7 @@
       <c r="O126" s="27"/>
       <c r="P126" s="27"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B127" s="27"/>
       <c r="C127" s="27"/>
       <c r="D127" s="27"/>
@@ -8526,7 +8550,7 @@
       <c r="O127" s="27"/>
       <c r="P127" s="27"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B128" s="27"/>
       <c r="C128" s="27"/>
       <c r="D128" s="27"/>
@@ -8543,7 +8567,7 @@
       <c r="O128" s="27"/>
       <c r="P128" s="27"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B129" s="27"/>
       <c r="C129" s="27"/>
       <c r="D129" s="27"/>
@@ -8560,7 +8584,7 @@
       <c r="O129" s="27"/>
       <c r="P129" s="27"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B130" s="27"/>
       <c r="C130" s="27"/>
       <c r="D130" s="27"/>
@@ -8577,7 +8601,7 @@
       <c r="O130" s="27"/>
       <c r="P130" s="27"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B131" s="27"/>
       <c r="C131" s="27"/>
       <c r="D131" s="27"/>
@@ -8594,7 +8618,7 @@
       <c r="O131" s="27"/>
       <c r="P131" s="27"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B132" s="27"/>
       <c r="C132" s="27"/>
       <c r="D132" s="27"/>
@@ -8611,7 +8635,7 @@
       <c r="O132" s="27"/>
       <c r="P132" s="27"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B133" s="27"/>
       <c r="C133" s="27"/>
       <c r="D133" s="27"/>
@@ -8628,7 +8652,7 @@
       <c r="O133" s="27"/>
       <c r="P133" s="27"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B134" s="27"/>
       <c r="C134" s="27"/>
       <c r="D134" s="27"/>
@@ -8645,7 +8669,7 @@
       <c r="O134" s="27"/>
       <c r="P134" s="27"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B135" s="27"/>
       <c r="C135" s="27"/>
       <c r="D135" s="27"/>
@@ -8662,7 +8686,7 @@
       <c r="O135" s="27"/>
       <c r="P135" s="27"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B136" s="27"/>
       <c r="C136" s="27"/>
       <c r="D136" s="27"/>
@@ -8679,7 +8703,7 @@
       <c r="O136" s="27"/>
       <c r="P136" s="27"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B137" s="27"/>
       <c r="C137" s="27"/>
       <c r="D137" s="27"/>
@@ -8696,7 +8720,7 @@
       <c r="O137" s="27"/>
       <c r="P137" s="27"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B138" s="27"/>
       <c r="C138" s="27"/>
       <c r="D138" s="27"/>
@@ -8713,7 +8737,7 @@
       <c r="O138" s="27"/>
       <c r="P138" s="27"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B139" s="27"/>
       <c r="C139" s="27"/>
       <c r="D139" s="27"/>
@@ -8730,7 +8754,7 @@
       <c r="O139" s="27"/>
       <c r="P139" s="27"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B140" s="27"/>
       <c r="C140" s="27"/>
       <c r="D140" s="27"/>
@@ -8747,7 +8771,7 @@
       <c r="O140" s="27"/>
       <c r="P140" s="27"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B141" s="27"/>
       <c r="C141" s="27"/>
       <c r="D141" s="27"/>
@@ -8764,7 +8788,7 @@
       <c r="O141" s="27"/>
       <c r="P141" s="27"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B142" s="27"/>
       <c r="C142" s="27"/>
       <c r="D142" s="27"/>
@@ -8781,7 +8805,7 @@
       <c r="O142" s="27"/>
       <c r="P142" s="27"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B143" s="27"/>
       <c r="C143" s="27"/>
       <c r="D143" s="27"/>
@@ -8798,7 +8822,7 @@
       <c r="O143" s="27"/>
       <c r="P143" s="27"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B144" s="27"/>
       <c r="C144" s="27"/>
       <c r="D144" s="27"/>
@@ -8815,7 +8839,7 @@
       <c r="O144" s="27"/>
       <c r="P144" s="27"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B145" s="27"/>
       <c r="C145" s="27"/>
       <c r="D145" s="27"/>
@@ -8832,7 +8856,7 @@
       <c r="O145" s="27"/>
       <c r="P145" s="27"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B146" s="27"/>
       <c r="C146" s="27"/>
       <c r="D146" s="27"/>
@@ -8849,7 +8873,7 @@
       <c r="O146" s="27"/>
       <c r="P146" s="27"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B147" s="27"/>
       <c r="C147" s="27"/>
       <c r="D147" s="27"/>
@@ -8866,7 +8890,7 @@
       <c r="O147" s="27"/>
       <c r="P147" s="27"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B148" s="27"/>
       <c r="C148" s="27"/>
       <c r="D148" s="27"/>
@@ -8883,7 +8907,7 @@
       <c r="O148" s="27"/>
       <c r="P148" s="27"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B149" s="27"/>
       <c r="C149" s="27"/>
       <c r="D149" s="27"/>
@@ -8900,7 +8924,7 @@
       <c r="O149" s="27"/>
       <c r="P149" s="27"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B150" s="27"/>
       <c r="C150" s="27"/>
       <c r="D150" s="27"/>
@@ -8917,7 +8941,7 @@
       <c r="O150" s="27"/>
       <c r="P150" s="27"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B151" s="27"/>
       <c r="C151" s="27"/>
       <c r="D151" s="27"/>
@@ -8934,7 +8958,7 @@
       <c r="O151" s="27"/>
       <c r="P151" s="27"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B152" s="27"/>
       <c r="C152" s="27"/>
       <c r="D152" s="27"/>
@@ -8951,7 +8975,7 @@
       <c r="O152" s="27"/>
       <c r="P152" s="27"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B153" s="27"/>
       <c r="C153" s="27"/>
       <c r="D153" s="27"/>
@@ -8968,7 +8992,7 @@
       <c r="O153" s="27"/>
       <c r="P153" s="27"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B154" s="27"/>
       <c r="C154" s="27"/>
       <c r="D154" s="27"/>
@@ -8985,7 +9009,7 @@
       <c r="O154" s="27"/>
       <c r="P154" s="27"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B155" s="27"/>
       <c r="C155" s="27"/>
       <c r="D155" s="27"/>
@@ -9002,7 +9026,7 @@
       <c r="O155" s="27"/>
       <c r="P155" s="27"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B156" s="27"/>
       <c r="C156" s="27"/>
       <c r="D156" s="27"/>
@@ -9019,7 +9043,7 @@
       <c r="O156" s="27"/>
       <c r="P156" s="27"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B157" s="27"/>
       <c r="C157" s="27"/>
       <c r="D157" s="27"/>
@@ -9036,7 +9060,7 @@
       <c r="O157" s="27"/>
       <c r="P157" s="27"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B158" s="27"/>
       <c r="C158" s="27"/>
       <c r="D158" s="27"/>
@@ -9053,7 +9077,7 @@
       <c r="O158" s="27"/>
       <c r="P158" s="27"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B159" s="27"/>
       <c r="C159" s="27"/>
       <c r="D159" s="27"/>
@@ -9070,7 +9094,7 @@
       <c r="O159" s="27"/>
       <c r="P159" s="27"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B160" s="27"/>
       <c r="C160" s="27"/>
       <c r="D160" s="27"/>
@@ -9096,21 +9120,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q99"/>
+  <dimension ref="A1:Q100"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K95" sqref="K95"/>
+      <selection pane="bottomLeft" activeCell="M106" sqref="M106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -9131,7 +9155,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -9152,7 +9176,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -9205,7 +9229,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -9258,7 +9282,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -9311,7 +9335,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -9364,7 +9388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -9417,7 +9441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -9470,7 +9494,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -9523,7 +9547,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -9576,7 +9600,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -9629,7 +9653,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -9682,7 +9706,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -9735,7 +9759,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -9788,7 +9812,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -9841,7 +9865,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -9894,7 +9918,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -9947,7 +9971,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -10000,7 +10024,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -10053,7 +10077,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -10106,7 +10130,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -10159,7 +10183,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -10212,7 +10236,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -10265,7 +10289,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -10318,7 +10342,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -10371,7 +10395,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -10424,7 +10448,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -10477,7 +10501,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -10530,7 +10554,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -10583,7 +10607,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -10636,7 +10660,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -10689,7 +10713,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -10742,7 +10766,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -10795,7 +10819,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -10848,7 +10872,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -10901,7 +10925,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="29">
         <v>43940</v>
       </c>
@@ -10954,7 +10978,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="29">
         <v>43941</v>
       </c>
@@ -11007,7 +11031,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="29">
         <v>43942</v>
       </c>
@@ -11060,7 +11084,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="29">
         <v>43943</v>
       </c>
@@ -11113,7 +11137,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="29">
         <v>43944</v>
       </c>
@@ -11166,7 +11190,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="29">
         <v>43945</v>
       </c>
@@ -11219,7 +11243,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="29">
         <v>43946</v>
       </c>
@@ -11272,7 +11296,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="29">
         <v>43947</v>
       </c>
@@ -11325,7 +11349,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="29">
         <v>43948</v>
       </c>
@@ -11378,7 +11402,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="29">
         <v>43949</v>
       </c>
@@ -11431,7 +11455,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="29">
         <v>43950</v>
       </c>
@@ -11484,7 +11508,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="29">
         <v>43951</v>
       </c>
@@ -11537,7 +11561,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="29">
         <v>43952</v>
       </c>
@@ -11590,7 +11614,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="29">
         <v>43953</v>
       </c>
@@ -11643,7 +11667,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="29">
         <v>43954</v>
       </c>
@@ -11696,7 +11720,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="29">
         <v>43955</v>
       </c>
@@ -11749,7 +11773,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="29">
         <v>43956</v>
       </c>
@@ -11802,7 +11826,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="29">
         <v>43957</v>
       </c>
@@ -11855,7 +11879,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="29">
         <v>43958</v>
       </c>
@@ -11908,7 +11932,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="29">
         <v>43959</v>
       </c>
@@ -11961,7 +11985,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="29">
         <v>43960</v>
       </c>
@@ -12014,7 +12038,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="29">
         <v>43961</v>
       </c>
@@ -12067,7 +12091,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="29">
         <v>43962</v>
       </c>
@@ -12120,7 +12144,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="29">
         <v>43963</v>
       </c>
@@ -12173,7 +12197,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="29">
         <v>43964</v>
       </c>
@@ -12226,7 +12250,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="29">
         <v>43965</v>
       </c>
@@ -12279,7 +12303,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="29">
         <v>43966</v>
       </c>
@@ -12332,7 +12356,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="29">
         <v>43967</v>
       </c>
@@ -12385,7 +12409,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="29">
         <v>43968</v>
       </c>
@@ -12438,7 +12462,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="29">
         <v>43969</v>
       </c>
@@ -12491,7 +12515,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="29">
         <v>43970</v>
       </c>
@@ -12544,7 +12568,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="29">
         <v>43971</v>
       </c>
@@ -12597,7 +12621,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="29">
         <v>43972</v>
       </c>
@@ -12650,7 +12674,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="29">
         <v>43973</v>
       </c>
@@ -12703,7 +12727,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="29">
         <v>43974</v>
       </c>
@@ -12756,7 +12780,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="29">
         <v>43975</v>
       </c>
@@ -12809,7 +12833,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="29">
         <v>43976</v>
       </c>
@@ -12862,7 +12886,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="29">
         <v>43977</v>
       </c>
@@ -12915,7 +12939,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="29">
         <v>43978</v>
       </c>
@@ -12968,7 +12992,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="29">
         <v>43979</v>
       </c>
@@ -13021,7 +13045,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="29">
         <v>43980</v>
       </c>
@@ -13074,7 +13098,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="29">
         <v>43981</v>
       </c>
@@ -13127,7 +13151,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="29">
         <v>43982</v>
       </c>
@@ -13180,7 +13204,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="29">
         <v>43983</v>
       </c>
@@ -13233,7 +13257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="29">
         <v>43984</v>
       </c>
@@ -13286,7 +13310,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A81" s="29">
         <v>43985</v>
       </c>
@@ -13339,7 +13363,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A82" s="29">
         <v>43986</v>
       </c>
@@ -13392,7 +13416,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A83" s="29">
         <v>43987</v>
       </c>
@@ -13445,7 +13469,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A84" s="29">
         <v>43988</v>
       </c>
@@ -13498,7 +13522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A85" s="29">
         <v>43989</v>
       </c>
@@ -13551,7 +13575,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A86" s="29">
         <v>43990</v>
       </c>
@@ -13604,7 +13628,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A87" s="29">
         <v>43991</v>
       </c>
@@ -13657,7 +13681,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A88" s="29">
         <v>43992</v>
       </c>
@@ -13710,7 +13734,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A89" s="29">
         <v>43993</v>
       </c>
@@ -13763,7 +13787,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A90" s="29">
         <v>43994</v>
       </c>
@@ -13816,7 +13840,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A91" s="29">
         <v>43995</v>
       </c>
@@ -13869,7 +13893,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A92" s="29">
         <v>43996</v>
       </c>
@@ -13922,7 +13946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" s="29">
         <v>43997</v>
       </c>
@@ -13975,7 +13999,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A94" s="29">
         <v>43998</v>
       </c>
@@ -14028,7 +14052,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A95" s="29">
         <v>43999</v>
       </c>
@@ -14081,7 +14105,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A96" s="29">
         <v>44000</v>
       </c>
@@ -14134,7 +14158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A97" s="29">
         <v>44001</v>
       </c>
@@ -14187,7 +14211,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A98" s="29">
         <v>44002</v>
       </c>
@@ -14240,7 +14264,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A99" s="29">
         <v>44003</v>
       </c>
@@ -14291,6 +14315,59 @@
       </c>
       <c r="Q99" s="13">
         <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A100" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K100" s="11">
+        <v>6</v>
+      </c>
+      <c r="L100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O100" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P100" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q100" s="13">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -14302,23 +14379,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R91"/>
+  <dimension ref="A1:R92"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Y94" sqref="Y94"/>
+      <selection pane="bottomRight" activeCell="L86" sqref="L86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="15.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -14339,7 +14416,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -14360,7 +14437,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -14413,7 +14490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -14466,7 +14543,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -14519,7 +14596,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -14572,7 +14649,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -14625,7 +14702,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -14678,7 +14755,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -14731,7 +14808,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -14784,7 +14861,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -14837,7 +14914,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -14890,7 +14967,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -14943,7 +15020,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -14996,7 +15073,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -15049,7 +15126,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -15102,7 +15179,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -15155,7 +15232,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -15208,7 +15285,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -15261,7 +15338,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -15314,7 +15391,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -15367,7 +15444,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -15420,7 +15497,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -15473,7 +15550,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -15526,7 +15603,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -15579,7 +15656,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -15632,7 +15709,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -15685,7 +15762,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -15738,7 +15815,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -15791,7 +15868,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -15844,7 +15921,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -15897,7 +15974,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -15950,7 +16027,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -16003,7 +16080,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -16056,7 +16133,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -16109,7 +16186,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="29">
         <v>43948</v>
       </c>
@@ -16162,7 +16239,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="29">
         <v>43949</v>
       </c>
@@ -16215,7 +16292,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="29">
         <v>43950</v>
       </c>
@@ -16268,7 +16345,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="29">
         <v>43951</v>
       </c>
@@ -16321,7 +16398,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="29">
         <v>43952</v>
       </c>
@@ -16374,7 +16451,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="29">
         <v>43953</v>
       </c>
@@ -16427,7 +16504,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="29">
         <v>43954</v>
       </c>
@@ -16480,7 +16557,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="29">
         <v>43955</v>
       </c>
@@ -16533,7 +16610,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="29">
         <v>43956</v>
       </c>
@@ -16586,7 +16663,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="29">
         <v>43957</v>
       </c>
@@ -16639,7 +16716,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="29">
         <v>43958</v>
       </c>
@@ -16692,7 +16769,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="29">
         <v>43959</v>
       </c>
@@ -16745,7 +16822,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="29">
         <v>43960</v>
       </c>
@@ -16798,7 +16875,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="29">
         <v>43961</v>
       </c>
@@ -16851,7 +16928,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="29">
         <v>43962</v>
       </c>
@@ -16904,7 +16981,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="29">
         <v>43963</v>
       </c>
@@ -16957,7 +17034,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="29">
         <v>43964</v>
       </c>
@@ -17010,7 +17087,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="29">
         <v>43965</v>
       </c>
@@ -17063,7 +17140,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="29">
         <v>43966</v>
       </c>
@@ -17116,7 +17193,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="29">
         <v>43967</v>
       </c>
@@ -17169,7 +17246,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="29">
         <v>43968</v>
       </c>
@@ -17222,7 +17299,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="29">
         <v>43969</v>
       </c>
@@ -17275,7 +17352,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="29">
         <v>43970</v>
       </c>
@@ -17328,7 +17405,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="29">
         <v>43971</v>
       </c>
@@ -17381,7 +17458,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="29">
         <v>43972</v>
       </c>
@@ -17434,7 +17511,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="29">
         <v>43973</v>
       </c>
@@ -17487,7 +17564,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="29">
         <v>43974</v>
       </c>
@@ -17540,7 +17617,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="29">
         <v>43975</v>
       </c>
@@ -17593,7 +17670,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="29">
         <v>43976</v>
       </c>
@@ -17646,7 +17723,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65" s="49">
         <v>43977</v>
       </c>
@@ -17699,7 +17776,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="49">
         <v>43978</v>
       </c>
@@ -17752,7 +17829,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67" s="49">
         <v>43979</v>
       </c>
@@ -17805,7 +17882,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68" s="49">
         <v>43980</v>
       </c>
@@ -17858,7 +17935,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69" s="49">
         <v>43981</v>
       </c>
@@ -17911,7 +17988,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70" s="49">
         <v>43982</v>
       </c>
@@ -17964,7 +18041,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71" s="49">
         <v>43983</v>
       </c>
@@ -18017,7 +18094,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72" s="49">
         <v>43984</v>
       </c>
@@ -18070,7 +18147,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73" s="49">
         <v>43985</v>
       </c>
@@ -18123,7 +18200,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74" s="49">
         <v>43986</v>
       </c>
@@ -18176,7 +18253,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75" s="49">
         <v>43987</v>
       </c>
@@ -18229,7 +18306,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76" s="49">
         <v>43988</v>
       </c>
@@ -18282,7 +18359,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77" s="49">
         <v>43989</v>
       </c>
@@ -18335,7 +18412,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78" s="49">
         <v>43990</v>
       </c>
@@ -18388,7 +18465,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79" s="49">
         <v>43991</v>
       </c>
@@ -18441,7 +18518,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80" s="49">
         <v>43992</v>
       </c>
@@ -18495,7 +18572,7 @@
       </c>
       <c r="R80" s="52"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="49">
         <v>43993</v>
       </c>
@@ -18549,7 +18626,7 @@
       </c>
       <c r="R81" s="52"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="49">
         <v>43994</v>
       </c>
@@ -18603,7 +18680,7 @@
       </c>
       <c r="R82" s="52"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="49">
         <v>43995</v>
       </c>
@@ -18656,7 +18733,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="49">
         <v>43996</v>
       </c>
@@ -18709,7 +18786,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="49">
         <v>43997</v>
       </c>
@@ -18762,7 +18839,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="49">
         <v>43998</v>
       </c>
@@ -18815,7 +18892,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="49">
         <v>43999</v>
       </c>
@@ -18868,7 +18945,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="49">
         <v>44000</v>
       </c>
@@ -18921,7 +18998,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="49">
         <v>44001</v>
       </c>
@@ -18974,7 +19051,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="49">
         <v>44002</v>
       </c>
@@ -19027,7 +19104,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="49">
         <v>44003</v>
       </c>
@@ -19078,6 +19155,59 @@
       </c>
       <c r="Q91" s="13">
         <v>518</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A92" s="49">
+        <v>44004</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E92" s="14">
+        <v>53</v>
+      </c>
+      <c r="F92" s="14">
+        <v>5</v>
+      </c>
+      <c r="G92" s="14">
+        <v>42</v>
+      </c>
+      <c r="H92" s="14">
+        <v>236</v>
+      </c>
+      <c r="I92" s="14">
+        <v>7</v>
+      </c>
+      <c r="J92" s="14">
+        <v>39</v>
+      </c>
+      <c r="K92" s="11">
+        <v>127</v>
+      </c>
+      <c r="L92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P92" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q92" s="13">
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -19089,23 +19219,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R91"/>
+  <dimension ref="A1:R92"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H95" sqref="H95"/>
+      <selection pane="bottomRight" activeCell="Q92" sqref="Q92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5703125" style="2"/>
+    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -19126,7 +19256,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -19147,7 +19277,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -19200,7 +19330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -19253,7 +19383,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -19306,7 +19436,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -19359,7 +19489,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -19412,7 +19542,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -19465,7 +19595,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -19518,7 +19648,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -19571,7 +19701,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -19624,7 +19754,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -19677,7 +19807,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -19730,7 +19860,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -19783,7 +19913,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -19836,7 +19966,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -19889,7 +20019,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -19942,7 +20072,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -19995,7 +20125,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -20048,7 +20178,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -20101,7 +20231,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -20154,7 +20284,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -20207,7 +20337,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -20260,7 +20390,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -20313,7 +20443,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -20366,7 +20496,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -20419,7 +20549,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -20472,7 +20602,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -20525,7 +20655,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -20578,7 +20708,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -20631,7 +20761,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -20684,7 +20814,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -20737,7 +20867,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -20790,7 +20920,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -20843,7 +20973,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -20896,7 +21026,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="29">
         <v>43948</v>
       </c>
@@ -20949,7 +21079,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="29">
         <v>43949</v>
       </c>
@@ -21002,7 +21132,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="29">
         <v>43950</v>
       </c>
@@ -21055,7 +21185,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="29">
         <v>43951</v>
       </c>
@@ -21108,7 +21238,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="29">
         <v>43952</v>
       </c>
@@ -21161,7 +21291,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="29">
         <v>43953</v>
       </c>
@@ -21214,7 +21344,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="29">
         <v>43954</v>
       </c>
@@ -21267,7 +21397,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43" s="29">
         <v>43955</v>
       </c>
@@ -21320,7 +21450,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44" s="29">
         <v>43956</v>
       </c>
@@ -21373,7 +21503,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="29">
         <v>43957</v>
       </c>
@@ -21426,7 +21556,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" s="29">
         <v>43958</v>
       </c>
@@ -21479,7 +21609,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" s="29">
         <v>43959</v>
       </c>
@@ -21532,7 +21662,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" s="29">
         <v>43960</v>
       </c>
@@ -21585,7 +21715,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A49" s="29">
         <v>43961</v>
       </c>
@@ -21638,7 +21768,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A50" s="29">
         <v>43962</v>
       </c>
@@ -21691,7 +21821,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="29">
         <v>43963</v>
       </c>
@@ -21744,7 +21874,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A52" s="29">
         <v>43964</v>
       </c>
@@ -21797,7 +21927,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A53" s="29">
         <v>43965</v>
       </c>
@@ -21850,7 +21980,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A54" s="29">
         <v>43966</v>
       </c>
@@ -21903,7 +22033,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" s="29">
         <v>43967</v>
       </c>
@@ -21956,7 +22086,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="29">
         <v>43968</v>
       </c>
@@ -22009,7 +22139,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="29">
         <v>43969</v>
       </c>
@@ -22062,7 +22192,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A58" s="29">
         <v>43970</v>
       </c>
@@ -22115,7 +22245,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A59" s="29">
         <v>43971</v>
       </c>
@@ -22168,7 +22298,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A60" s="29">
         <v>43972</v>
       </c>
@@ -22221,7 +22351,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="29">
         <v>43973</v>
       </c>
@@ -22274,7 +22404,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="29">
         <v>43974</v>
       </c>
@@ -22327,7 +22457,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A63" s="29">
         <v>43975</v>
       </c>
@@ -22380,7 +22510,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A64" s="29">
         <v>43976</v>
       </c>
@@ -22433,7 +22563,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A65" s="29">
         <v>43977</v>
       </c>
@@ -22486,7 +22616,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A66" s="29">
         <v>43978</v>
       </c>
@@ -22539,7 +22669,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A67" s="29">
         <v>43979</v>
       </c>
@@ -22592,7 +22722,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A68" s="29">
         <v>43980</v>
       </c>
@@ -22645,7 +22775,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A69" s="29">
         <v>43981</v>
       </c>
@@ -22698,7 +22828,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A70" s="29">
         <v>43982</v>
       </c>
@@ -22751,7 +22881,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A71" s="29">
         <v>43983</v>
       </c>
@@ -22804,7 +22934,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A72" s="29">
         <v>43984</v>
       </c>
@@ -22857,7 +22987,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A73" s="29">
         <v>43985</v>
       </c>
@@ -22910,7 +23040,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A74" s="29">
         <v>43986</v>
       </c>
@@ -22963,7 +23093,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A75" s="29">
         <v>43987</v>
       </c>
@@ -23016,7 +23146,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A76" s="29">
         <v>43988</v>
       </c>
@@ -23069,7 +23199,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A77" s="29">
         <v>43989</v>
       </c>
@@ -23122,7 +23252,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" s="29">
         <v>43990</v>
       </c>
@@ -23175,7 +23305,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A79" s="29">
         <v>43991</v>
       </c>
@@ -23228,7 +23358,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A80" s="29">
         <v>43992</v>
       </c>
@@ -23281,7 +23411,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81" s="29">
         <v>43993</v>
       </c>
@@ -23334,7 +23464,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82" s="29">
         <v>43994</v>
       </c>
@@ -23387,7 +23517,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83" s="29">
         <v>43995</v>
       </c>
@@ -23440,7 +23570,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84" s="29">
         <v>43996</v>
       </c>
@@ -23493,7 +23623,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85" s="29">
         <v>43997</v>
       </c>
@@ -23546,7 +23676,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86" s="29">
         <v>43998</v>
       </c>
@@ -23599,7 +23729,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87" s="29">
         <v>43999</v>
       </c>
@@ -23652,7 +23782,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88" s="29">
         <v>44000</v>
       </c>
@@ -23705,7 +23835,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89" s="29">
         <v>44001</v>
       </c>
@@ -23758,7 +23888,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90" s="29">
         <v>44002</v>
       </c>
@@ -23811,7 +23941,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91" s="29">
         <v>44003</v>
       </c>
@@ -23864,6 +23994,59 @@
         <v>283</v>
       </c>
       <c r="R91" s="52"/>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A92" s="29">
+        <v>44004</v>
+      </c>
+      <c r="B92" s="11">
+        <v>17</v>
+      </c>
+      <c r="C92" s="11">
+        <v>25</v>
+      </c>
+      <c r="D92" s="11">
+        <v>6</v>
+      </c>
+      <c r="E92" s="11">
+        <v>20</v>
+      </c>
+      <c r="F92" s="11">
+        <v>26</v>
+      </c>
+      <c r="G92" s="11">
+        <v>10</v>
+      </c>
+      <c r="H92" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I92" s="11">
+        <v>30</v>
+      </c>
+      <c r="J92" s="11">
+        <v>48</v>
+      </c>
+      <c r="K92" s="11">
+        <v>160</v>
+      </c>
+      <c r="L92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N92" s="11">
+        <v>7</v>
+      </c>
+      <c r="O92" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P92" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q92" s="13">
+        <v>352</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -23896,7 +24079,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-21T11:36:26Z</value>
+      <value order="0">2020-06-22T12:09:14Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -23911,13 +24094,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41865896</value>
+      <value order="0">vA41884158</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">27.8</value>
+      <value order="0">27.10</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">207</value>
+      <value order="0">209</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-23 20:08) (#165)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -2770,10 +2770,10 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B94" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B91" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C114" sqref="C114"/>
+      <selection pane="bottomRight" activeCell="K116" sqref="K116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8279,21 +8279,54 @@
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B112" s="27"/>
-      <c r="C112" s="27"/>
-      <c r="D112" s="27"/>
-      <c r="E112" s="27"/>
-      <c r="F112" s="27"/>
-      <c r="G112" s="27"/>
-      <c r="H112" s="27"/>
-      <c r="I112" s="27"/>
-      <c r="J112" s="27"/>
-      <c r="K112" s="27"/>
-      <c r="L112" s="27"/>
-      <c r="M112" s="27"/>
-      <c r="N112" s="27"/>
-      <c r="O112" s="27"/>
-      <c r="P112" s="27"/>
+      <c r="A112" s="5">
+        <v>44005</v>
+      </c>
+      <c r="B112" s="27">
+        <v>1251</v>
+      </c>
+      <c r="C112" s="27">
+        <v>346</v>
+      </c>
+      <c r="D112" s="27">
+        <v>285</v>
+      </c>
+      <c r="E112" s="27">
+        <v>928</v>
+      </c>
+      <c r="F112" s="27">
+        <v>1058</v>
+      </c>
+      <c r="G112" s="27">
+        <v>1413</v>
+      </c>
+      <c r="H112" s="27">
+        <v>4832</v>
+      </c>
+      <c r="I112" s="27">
+        <v>374</v>
+      </c>
+      <c r="J112" s="27">
+        <v>2715</v>
+      </c>
+      <c r="K112" s="27">
+        <v>3147</v>
+      </c>
+      <c r="L112" s="27">
+        <v>9</v>
+      </c>
+      <c r="M112" s="27">
+        <v>54</v>
+      </c>
+      <c r="N112" s="27">
+        <v>1763</v>
+      </c>
+      <c r="O112" s="27">
+        <v>7</v>
+      </c>
+      <c r="P112" s="31">
+        <v>18182</v>
+      </c>
     </row>
     <row r="113" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B113" s="27"/>
@@ -9120,11 +9153,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q100"/>
+  <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M106" sqref="M106"/>
+      <selection pane="bottomLeft" activeCell="L100" sqref="L100:P101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14370,6 +14403,59 @@
         <v>15</v>
       </c>
     </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A101" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="K101" s="11">
+        <v>10</v>
+      </c>
+      <c r="L101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O101" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P101" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q101" s="13">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -14379,13 +14465,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R92"/>
+  <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L86" sqref="L86"/>
+      <selection pane="bottomRight" activeCell="S82" sqref="S82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19210,6 +19296,59 @@
         <v>515</v>
       </c>
     </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A93" s="49">
+        <v>44005</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E93" s="11">
+        <v>53</v>
+      </c>
+      <c r="F93" s="11">
+        <v>5</v>
+      </c>
+      <c r="G93" s="11">
+        <v>43</v>
+      </c>
+      <c r="H93" s="11">
+        <v>237</v>
+      </c>
+      <c r="I93" s="11">
+        <v>7</v>
+      </c>
+      <c r="J93" s="11">
+        <v>37</v>
+      </c>
+      <c r="K93" s="11">
+        <v>123</v>
+      </c>
+      <c r="L93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N93" s="11">
+        <v>5</v>
+      </c>
+      <c r="O93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P93" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q93" s="11">
+        <v>512</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
@@ -19219,13 +19358,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R92"/>
+  <dimension ref="A1:R93"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q92" sqref="Q92"/>
+      <selection pane="bottomRight" activeCell="K89" sqref="K89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24046,6 +24185,59 @@
       </c>
       <c r="Q92" s="13">
         <v>352</v>
+      </c>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A93" s="29">
+        <v>44005</v>
+      </c>
+      <c r="B93" s="11">
+        <v>21</v>
+      </c>
+      <c r="C93" s="11">
+        <v>20</v>
+      </c>
+      <c r="D93" s="11">
+        <v>20</v>
+      </c>
+      <c r="E93" s="11">
+        <v>12</v>
+      </c>
+      <c r="F93" s="11">
+        <v>25</v>
+      </c>
+      <c r="G93" s="11">
+        <v>15</v>
+      </c>
+      <c r="H93" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I93" s="11">
+        <v>18</v>
+      </c>
+      <c r="J93" s="11">
+        <v>56</v>
+      </c>
+      <c r="K93" s="11">
+        <v>155</v>
+      </c>
+      <c r="L93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N93" s="11">
+        <v>11</v>
+      </c>
+      <c r="O93" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P93" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q93" s="13">
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -24079,7 +24271,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-22T12:09:14Z</value>
+      <value order="0">2020-06-23T11:53:43Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -24094,13 +24286,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41884158</value>
+      <value order="0">vA41913469</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">27.10</value>
+      <value order="0">27.12</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">209</value>
+      <value order="0">211</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-24 20:08) (#174)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U445783\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA18464\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u419207\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA10434\A28088333\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5988" windowHeight="6048" tabRatio="803" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6050" tabRatio="803" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2097" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -2662,21 +2662,21 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.44140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.44140625" style="2"/>
+    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.453125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -2692,13 +2692,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -2706,7 +2706,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -2750,12 +2750,12 @@
       <selection activeCell="O81" sqref="O81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.44140625" style="2"/>
+    <col min="1" max="16384" width="9.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="42"/>
     </row>
   </sheetData>
@@ -2770,20 +2770,20 @@
   <dimension ref="A1:S160"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K116" sqref="K116"/>
+      <selection pane="bottomRight" activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.44140625" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.5546875" style="2"/>
+    <col min="2" max="16" width="11.453125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2803,7 +2803,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -2822,7 +2822,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -2922,7 +2922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -3422,7 +3422,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -3522,7 +3522,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -3972,7 +3972,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -4322,7 +4322,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -4522,7 +4522,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -4572,7 +4572,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -4722,7 +4722,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -4772,7 +4772,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -4972,7 +4972,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -5122,7 +5122,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -5222,7 +5222,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -5423,7 +5423,7 @@
       </c>
       <c r="R54" s="37"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -5474,7 +5474,7 @@
       </c>
       <c r="R55" s="37"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -5525,7 +5525,7 @@
       </c>
       <c r="R56" s="38"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -5575,7 +5575,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -5626,7 +5626,7 @@
       </c>
       <c r="R58" s="37"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -5678,7 +5678,7 @@
       <c r="R59" s="37"/>
       <c r="S59" s="37"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -5828,7 +5828,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -5928,7 +5928,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -5978,7 +5978,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -6028,7 +6028,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -6078,7 +6078,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -6378,7 +6378,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -6428,7 +6428,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -6478,7 +6478,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -6578,7 +6578,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -6628,7 +6628,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -6728,7 +6728,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -6828,7 +6828,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -6878,7 +6878,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -6928,7 +6928,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -6978,7 +6978,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -7028,7 +7028,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -7228,7 +7228,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -7278,7 +7278,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -7328,7 +7328,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -7378,7 +7378,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -7428,7 +7428,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -7478,7 +7478,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -7528,7 +7528,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" s="5">
         <v>43991</v>
       </c>
@@ -7628,7 +7628,7 @@
         <v>15653</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99" s="5">
         <v>43992</v>
       </c>
@@ -7678,7 +7678,7 @@
         <v>15665</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100" s="5">
         <v>43993</v>
       </c>
@@ -7728,7 +7728,7 @@
         <v>15682</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101" s="5">
         <v>43994</v>
       </c>
@@ -7778,7 +7778,7 @@
         <v>15709</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102" s="5">
         <v>43995</v>
       </c>
@@ -7828,7 +7828,7 @@
         <v>15730</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103" s="53">
         <v>43996</v>
       </c>
@@ -7878,7 +7878,7 @@
         <v>15755</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="5">
         <v>43997</v>
       </c>
@@ -7928,7 +7928,7 @@
         <v>18030</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A105" s="5">
         <v>43998</v>
       </c>
@@ -7978,7 +7978,7 @@
         <v>18045</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A106" s="5">
         <v>43999</v>
       </c>
@@ -8028,7 +8028,7 @@
         <v>18066</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A107" s="5">
         <v>44000</v>
       </c>
@@ -8078,7 +8078,7 @@
         <v>18077</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A108" s="5">
         <v>44001</v>
       </c>
@@ -8128,7 +8128,7 @@
         <v>18104</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A109" s="5">
         <v>44002</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>18130</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A110" s="5">
         <v>44003</v>
       </c>
@@ -8228,7 +8228,7 @@
         <v>18156</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A111" s="5">
         <v>44004</v>
       </c>
@@ -8278,7 +8278,7 @@
         <v>18170</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A112" s="5">
         <v>44005</v>
       </c>
@@ -8328,24 +8328,57 @@
         <v>18182</v>
       </c>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B113" s="27"/>
-      <c r="C113" s="27"/>
-      <c r="D113" s="27"/>
-      <c r="E113" s="27"/>
-      <c r="F113" s="27"/>
-      <c r="G113" s="27"/>
-      <c r="H113" s="27"/>
-      <c r="I113" s="27"/>
-      <c r="J113" s="27"/>
-      <c r="K113" s="27"/>
-      <c r="L113" s="27"/>
-      <c r="M113" s="27"/>
-      <c r="N113" s="27"/>
-      <c r="O113" s="27"/>
-      <c r="P113" s="27"/>
-    </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A113" s="5">
+        <v>44006</v>
+      </c>
+      <c r="B113" s="27">
+        <v>1251</v>
+      </c>
+      <c r="C113" s="27">
+        <v>346</v>
+      </c>
+      <c r="D113" s="27">
+        <v>285</v>
+      </c>
+      <c r="E113" s="27">
+        <v>928</v>
+      </c>
+      <c r="F113" s="27">
+        <v>1061</v>
+      </c>
+      <c r="G113" s="27">
+        <v>1413</v>
+      </c>
+      <c r="H113" s="27">
+        <v>4834</v>
+      </c>
+      <c r="I113" s="27">
+        <v>374</v>
+      </c>
+      <c r="J113" s="27">
+        <v>2715</v>
+      </c>
+      <c r="K113" s="27">
+        <v>3150</v>
+      </c>
+      <c r="L113" s="27">
+        <v>9</v>
+      </c>
+      <c r="M113" s="27">
+        <v>54</v>
+      </c>
+      <c r="N113" s="27">
+        <v>1764</v>
+      </c>
+      <c r="O113" s="27">
+        <v>7</v>
+      </c>
+      <c r="P113" s="31">
+        <v>18191</v>
+      </c>
+    </row>
+    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B114" s="27"/>
       <c r="C114" s="27"/>
       <c r="D114" s="27"/>
@@ -8362,7 +8395,7 @@
       <c r="O114" s="27"/>
       <c r="P114" s="27"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B115" s="27"/>
       <c r="C115" s="27"/>
       <c r="D115" s="27"/>
@@ -8379,7 +8412,7 @@
       <c r="O115" s="27"/>
       <c r="P115" s="27"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B116" s="27"/>
       <c r="C116" s="27"/>
       <c r="D116" s="27"/>
@@ -8396,7 +8429,7 @@
       <c r="O116" s="27"/>
       <c r="P116" s="27"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B117" s="27"/>
       <c r="C117" s="27"/>
       <c r="D117" s="27"/>
@@ -8413,7 +8446,7 @@
       <c r="O117" s="27"/>
       <c r="P117" s="27"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B118" s="27"/>
       <c r="C118" s="27"/>
       <c r="D118" s="27"/>
@@ -8430,7 +8463,7 @@
       <c r="O118" s="27"/>
       <c r="P118" s="27"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B119" s="27"/>
       <c r="C119" s="27"/>
       <c r="D119" s="27"/>
@@ -8447,7 +8480,7 @@
       <c r="O119" s="27"/>
       <c r="P119" s="27"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B120" s="27"/>
       <c r="C120" s="27"/>
       <c r="D120" s="27"/>
@@ -8464,7 +8497,7 @@
       <c r="O120" s="27"/>
       <c r="P120" s="27"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B121" s="27"/>
       <c r="C121" s="27"/>
       <c r="D121" s="27"/>
@@ -8481,7 +8514,7 @@
       <c r="O121" s="27"/>
       <c r="P121" s="27"/>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B122" s="27"/>
       <c r="C122" s="27"/>
       <c r="D122" s="27"/>
@@ -8498,7 +8531,7 @@
       <c r="O122" s="27"/>
       <c r="P122" s="27"/>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B123" s="27"/>
       <c r="C123" s="27"/>
       <c r="D123" s="27"/>
@@ -8515,7 +8548,7 @@
       <c r="O123" s="27"/>
       <c r="P123" s="27"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B124" s="27"/>
       <c r="C124" s="27"/>
       <c r="D124" s="27"/>
@@ -8532,7 +8565,7 @@
       <c r="O124" s="27"/>
       <c r="P124" s="27"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B125" s="27"/>
       <c r="C125" s="27"/>
       <c r="D125" s="27"/>
@@ -8549,7 +8582,7 @@
       <c r="O125" s="27"/>
       <c r="P125" s="27"/>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B126" s="27"/>
       <c r="C126" s="27"/>
       <c r="D126" s="27"/>
@@ -8566,7 +8599,7 @@
       <c r="O126" s="27"/>
       <c r="P126" s="27"/>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B127" s="27"/>
       <c r="C127" s="27"/>
       <c r="D127" s="27"/>
@@ -8583,7 +8616,7 @@
       <c r="O127" s="27"/>
       <c r="P127" s="27"/>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B128" s="27"/>
       <c r="C128" s="27"/>
       <c r="D128" s="27"/>
@@ -8600,7 +8633,7 @@
       <c r="O128" s="27"/>
       <c r="P128" s="27"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B129" s="27"/>
       <c r="C129" s="27"/>
       <c r="D129" s="27"/>
@@ -8617,7 +8650,7 @@
       <c r="O129" s="27"/>
       <c r="P129" s="27"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B130" s="27"/>
       <c r="C130" s="27"/>
       <c r="D130" s="27"/>
@@ -8634,7 +8667,7 @@
       <c r="O130" s="27"/>
       <c r="P130" s="27"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B131" s="27"/>
       <c r="C131" s="27"/>
       <c r="D131" s="27"/>
@@ -8651,7 +8684,7 @@
       <c r="O131" s="27"/>
       <c r="P131" s="27"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B132" s="27"/>
       <c r="C132" s="27"/>
       <c r="D132" s="27"/>
@@ -8668,7 +8701,7 @@
       <c r="O132" s="27"/>
       <c r="P132" s="27"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B133" s="27"/>
       <c r="C133" s="27"/>
       <c r="D133" s="27"/>
@@ -8685,7 +8718,7 @@
       <c r="O133" s="27"/>
       <c r="P133" s="27"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B134" s="27"/>
       <c r="C134" s="27"/>
       <c r="D134" s="27"/>
@@ -8702,7 +8735,7 @@
       <c r="O134" s="27"/>
       <c r="P134" s="27"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B135" s="27"/>
       <c r="C135" s="27"/>
       <c r="D135" s="27"/>
@@ -8719,7 +8752,7 @@
       <c r="O135" s="27"/>
       <c r="P135" s="27"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B136" s="27"/>
       <c r="C136" s="27"/>
       <c r="D136" s="27"/>
@@ -8736,7 +8769,7 @@
       <c r="O136" s="27"/>
       <c r="P136" s="27"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B137" s="27"/>
       <c r="C137" s="27"/>
       <c r="D137" s="27"/>
@@ -8753,7 +8786,7 @@
       <c r="O137" s="27"/>
       <c r="P137" s="27"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B138" s="27"/>
       <c r="C138" s="27"/>
       <c r="D138" s="27"/>
@@ -8770,7 +8803,7 @@
       <c r="O138" s="27"/>
       <c r="P138" s="27"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B139" s="27"/>
       <c r="C139" s="27"/>
       <c r="D139" s="27"/>
@@ -8787,7 +8820,7 @@
       <c r="O139" s="27"/>
       <c r="P139" s="27"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B140" s="27"/>
       <c r="C140" s="27"/>
       <c r="D140" s="27"/>
@@ -8804,7 +8837,7 @@
       <c r="O140" s="27"/>
       <c r="P140" s="27"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B141" s="27"/>
       <c r="C141" s="27"/>
       <c r="D141" s="27"/>
@@ -8821,7 +8854,7 @@
       <c r="O141" s="27"/>
       <c r="P141" s="27"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B142" s="27"/>
       <c r="C142" s="27"/>
       <c r="D142" s="27"/>
@@ -8838,7 +8871,7 @@
       <c r="O142" s="27"/>
       <c r="P142" s="27"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B143" s="27"/>
       <c r="C143" s="27"/>
       <c r="D143" s="27"/>
@@ -8855,7 +8888,7 @@
       <c r="O143" s="27"/>
       <c r="P143" s="27"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B144" s="27"/>
       <c r="C144" s="27"/>
       <c r="D144" s="27"/>
@@ -8872,7 +8905,7 @@
       <c r="O144" s="27"/>
       <c r="P144" s="27"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B145" s="27"/>
       <c r="C145" s="27"/>
       <c r="D145" s="27"/>
@@ -8889,7 +8922,7 @@
       <c r="O145" s="27"/>
       <c r="P145" s="27"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B146" s="27"/>
       <c r="C146" s="27"/>
       <c r="D146" s="27"/>
@@ -8906,7 +8939,7 @@
       <c r="O146" s="27"/>
       <c r="P146" s="27"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B147" s="27"/>
       <c r="C147" s="27"/>
       <c r="D147" s="27"/>
@@ -8923,7 +8956,7 @@
       <c r="O147" s="27"/>
       <c r="P147" s="27"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B148" s="27"/>
       <c r="C148" s="27"/>
       <c r="D148" s="27"/>
@@ -8940,7 +8973,7 @@
       <c r="O148" s="27"/>
       <c r="P148" s="27"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B149" s="27"/>
       <c r="C149" s="27"/>
       <c r="D149" s="27"/>
@@ -8957,7 +8990,7 @@
       <c r="O149" s="27"/>
       <c r="P149" s="27"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B150" s="27"/>
       <c r="C150" s="27"/>
       <c r="D150" s="27"/>
@@ -8974,7 +9007,7 @@
       <c r="O150" s="27"/>
       <c r="P150" s="27"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B151" s="27"/>
       <c r="C151" s="27"/>
       <c r="D151" s="27"/>
@@ -8991,7 +9024,7 @@
       <c r="O151" s="27"/>
       <c r="P151" s="27"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B152" s="27"/>
       <c r="C152" s="27"/>
       <c r="D152" s="27"/>
@@ -9008,7 +9041,7 @@
       <c r="O152" s="27"/>
       <c r="P152" s="27"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B153" s="27"/>
       <c r="C153" s="27"/>
       <c r="D153" s="27"/>
@@ -9025,7 +9058,7 @@
       <c r="O153" s="27"/>
       <c r="P153" s="27"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B154" s="27"/>
       <c r="C154" s="27"/>
       <c r="D154" s="27"/>
@@ -9042,7 +9075,7 @@
       <c r="O154" s="27"/>
       <c r="P154" s="27"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B155" s="27"/>
       <c r="C155" s="27"/>
       <c r="D155" s="27"/>
@@ -9059,7 +9092,7 @@
       <c r="O155" s="27"/>
       <c r="P155" s="27"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B156" s="27"/>
       <c r="C156" s="27"/>
       <c r="D156" s="27"/>
@@ -9076,7 +9109,7 @@
       <c r="O156" s="27"/>
       <c r="P156" s="27"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B157" s="27"/>
       <c r="C157" s="27"/>
       <c r="D157" s="27"/>
@@ -9093,7 +9126,7 @@
       <c r="O157" s="27"/>
       <c r="P157" s="27"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B158" s="27"/>
       <c r="C158" s="27"/>
       <c r="D158" s="27"/>
@@ -9110,7 +9143,7 @@
       <c r="O158" s="27"/>
       <c r="P158" s="27"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B159" s="27"/>
       <c r="C159" s="27"/>
       <c r="D159" s="27"/>
@@ -9127,7 +9160,7 @@
       <c r="O159" s="27"/>
       <c r="P159" s="27"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B160" s="27"/>
       <c r="C160" s="27"/>
       <c r="D160" s="27"/>
@@ -9153,21 +9186,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q101"/>
+  <dimension ref="A1:Q102"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L100" sqref="L100:P101"/>
+      <pane ySplit="3" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q103" sqref="Q103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -9188,7 +9221,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -9209,7 +9242,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -9262,7 +9295,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -9315,7 +9348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -9368,7 +9401,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -9421,7 +9454,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -9474,7 +9507,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -9527,7 +9560,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -9580,7 +9613,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -9633,7 +9666,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -9686,7 +9719,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -9739,7 +9772,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -9792,7 +9825,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -9845,7 +9878,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -9898,7 +9931,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -9951,7 +9984,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -10004,7 +10037,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -10057,7 +10090,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -10110,7 +10143,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -10163,7 +10196,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -10216,7 +10249,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -10269,7 +10302,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -10322,7 +10355,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -10375,7 +10408,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -10428,7 +10461,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -10481,7 +10514,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -10534,7 +10567,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -10587,7 +10620,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -10640,7 +10673,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -10693,7 +10726,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -10746,7 +10779,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -10799,7 +10832,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -10852,7 +10885,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -10905,7 +10938,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -10958,7 +10991,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="29">
         <v>43940</v>
       </c>
@@ -11011,7 +11044,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="29">
         <v>43941</v>
       </c>
@@ -11064,7 +11097,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="29">
         <v>43942</v>
       </c>
@@ -11117,7 +11150,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="29">
         <v>43943</v>
       </c>
@@ -11170,7 +11203,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="29">
         <v>43944</v>
       </c>
@@ -11223,7 +11256,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="29">
         <v>43945</v>
       </c>
@@ -11276,7 +11309,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="29">
         <v>43946</v>
       </c>
@@ -11329,7 +11362,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="29">
         <v>43947</v>
       </c>
@@ -11382,7 +11415,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="29">
         <v>43948</v>
       </c>
@@ -11435,7 +11468,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="29">
         <v>43949</v>
       </c>
@@ -11488,7 +11521,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="29">
         <v>43950</v>
       </c>
@@ -11541,7 +11574,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="29">
         <v>43951</v>
       </c>
@@ -11594,7 +11627,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="29">
         <v>43952</v>
       </c>
@@ -11647,7 +11680,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="29">
         <v>43953</v>
       </c>
@@ -11700,7 +11733,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="29">
         <v>43954</v>
       </c>
@@ -11753,7 +11786,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="29">
         <v>43955</v>
       </c>
@@ -11806,7 +11839,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="29">
         <v>43956</v>
       </c>
@@ -11859,7 +11892,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="29">
         <v>43957</v>
       </c>
@@ -11912,7 +11945,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="29">
         <v>43958</v>
       </c>
@@ -11965,7 +11998,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="29">
         <v>43959</v>
       </c>
@@ -12018,7 +12051,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="29">
         <v>43960</v>
       </c>
@@ -12071,7 +12104,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="29">
         <v>43961</v>
       </c>
@@ -12124,7 +12157,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="29">
         <v>43962</v>
       </c>
@@ -12177,7 +12210,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="29">
         <v>43963</v>
       </c>
@@ -12230,7 +12263,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="29">
         <v>43964</v>
       </c>
@@ -12283,7 +12316,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="29">
         <v>43965</v>
       </c>
@@ -12336,7 +12369,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="29">
         <v>43966</v>
       </c>
@@ -12389,7 +12422,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="29">
         <v>43967</v>
       </c>
@@ -12442,7 +12475,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="29">
         <v>43968</v>
       </c>
@@ -12495,7 +12528,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="29">
         <v>43969</v>
       </c>
@@ -12548,7 +12581,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="29">
         <v>43970</v>
       </c>
@@ -12601,7 +12634,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="29">
         <v>43971</v>
       </c>
@@ -12654,7 +12687,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="29">
         <v>43972</v>
       </c>
@@ -12707,7 +12740,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="29">
         <v>43973</v>
       </c>
@@ -12760,7 +12793,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="29">
         <v>43974</v>
       </c>
@@ -12813,7 +12846,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="29">
         <v>43975</v>
       </c>
@@ -12866,7 +12899,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="29">
         <v>43976</v>
       </c>
@@ -12919,7 +12952,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="29">
         <v>43977</v>
       </c>
@@ -12972,7 +13005,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="29">
         <v>43978</v>
       </c>
@@ -13025,7 +13058,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="29">
         <v>43979</v>
       </c>
@@ -13078,7 +13111,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="29">
         <v>43980</v>
       </c>
@@ -13131,7 +13164,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="29">
         <v>43981</v>
       </c>
@@ -13184,7 +13217,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="29">
         <v>43982</v>
       </c>
@@ -13237,7 +13270,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="29">
         <v>43983</v>
       </c>
@@ -13290,7 +13323,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="29">
         <v>43984</v>
       </c>
@@ -13343,7 +13376,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="29">
         <v>43985</v>
       </c>
@@ -13396,7 +13429,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="29">
         <v>43986</v>
       </c>
@@ -13449,7 +13482,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="29">
         <v>43987</v>
       </c>
@@ -13502,7 +13535,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="29">
         <v>43988</v>
       </c>
@@ -13555,7 +13588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" s="29">
         <v>43989</v>
       </c>
@@ -13608,7 +13641,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" s="29">
         <v>43990</v>
       </c>
@@ -13661,7 +13694,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" s="29">
         <v>43991</v>
       </c>
@@ -13714,7 +13747,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88" s="29">
         <v>43992</v>
       </c>
@@ -13767,7 +13800,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89" s="29">
         <v>43993</v>
       </c>
@@ -13820,7 +13853,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A90" s="29">
         <v>43994</v>
       </c>
@@ -13873,7 +13906,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A91" s="29">
         <v>43995</v>
       </c>
@@ -13926,7 +13959,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92" s="29">
         <v>43996</v>
       </c>
@@ -13979,7 +14012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A93" s="29">
         <v>43997</v>
       </c>
@@ -14032,7 +14065,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A94" s="29">
         <v>43998</v>
       </c>
@@ -14085,7 +14118,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95" s="29">
         <v>43999</v>
       </c>
@@ -14138,7 +14171,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96" s="29">
         <v>44000</v>
       </c>
@@ -14191,7 +14224,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A97" s="29">
         <v>44001</v>
       </c>
@@ -14244,7 +14277,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A98" s="29">
         <v>44002</v>
       </c>
@@ -14297,7 +14330,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A99" s="29">
         <v>44003</v>
       </c>
@@ -14350,7 +14383,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A100" s="29">
         <v>44004</v>
       </c>
@@ -14403,7 +14436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A101" s="29">
         <v>44005</v>
       </c>
@@ -14454,6 +14487,59 @@
       </c>
       <c r="Q101" s="13">
         <v>21</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A102" s="29">
+        <v>44006</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C102" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E102" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F102" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G102" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H102" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I102" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J102" s="14">
+        <v>6</v>
+      </c>
+      <c r="K102" s="11">
+        <v>7</v>
+      </c>
+      <c r="L102" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M102" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N102" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O102" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P102" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q102" s="13">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -14465,23 +14551,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R93"/>
+  <dimension ref="A1:R94"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S82" sqref="S82"/>
+      <selection pane="bottomRight" activeCell="P90" sqref="P90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="15.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -14502,7 +14588,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -14523,7 +14609,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -14576,7 +14662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -14629,7 +14715,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -14682,7 +14768,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -14735,7 +14821,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -14788,7 +14874,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -14841,7 +14927,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -14894,7 +14980,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -14947,7 +15033,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -15000,7 +15086,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -15053,7 +15139,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -15106,7 +15192,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -15159,7 +15245,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -15212,7 +15298,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -15265,7 +15351,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -15318,7 +15404,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -15371,7 +15457,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -15424,7 +15510,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -15477,7 +15563,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -15530,7 +15616,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -15583,7 +15669,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -15636,7 +15722,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -15689,7 +15775,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -15742,7 +15828,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -15795,7 +15881,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -15848,7 +15934,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -15901,7 +15987,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -15954,7 +16040,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -16007,7 +16093,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -16060,7 +16146,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -16113,7 +16199,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -16166,7 +16252,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -16219,7 +16305,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -16272,7 +16358,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="29">
         <v>43948</v>
       </c>
@@ -16325,7 +16411,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="29">
         <v>43949</v>
       </c>
@@ -16378,7 +16464,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="29">
         <v>43950</v>
       </c>
@@ -16431,7 +16517,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="29">
         <v>43951</v>
       </c>
@@ -16484,7 +16570,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="29">
         <v>43952</v>
       </c>
@@ -16537,7 +16623,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="29">
         <v>43953</v>
       </c>
@@ -16590,7 +16676,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="29">
         <v>43954</v>
       </c>
@@ -16643,7 +16729,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="29">
         <v>43955</v>
       </c>
@@ -16696,7 +16782,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="29">
         <v>43956</v>
       </c>
@@ -16749,7 +16835,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="29">
         <v>43957</v>
       </c>
@@ -16802,7 +16888,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="29">
         <v>43958</v>
       </c>
@@ -16855,7 +16941,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="29">
         <v>43959</v>
       </c>
@@ -16908,7 +16994,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="29">
         <v>43960</v>
       </c>
@@ -16961,7 +17047,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="29">
         <v>43961</v>
       </c>
@@ -17014,7 +17100,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="29">
         <v>43962</v>
       </c>
@@ -17067,7 +17153,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="29">
         <v>43963</v>
       </c>
@@ -17120,7 +17206,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="29">
         <v>43964</v>
       </c>
@@ -17173,7 +17259,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="29">
         <v>43965</v>
       </c>
@@ -17226,7 +17312,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="29">
         <v>43966</v>
       </c>
@@ -17279,7 +17365,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="29">
         <v>43967</v>
       </c>
@@ -17332,7 +17418,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="29">
         <v>43968</v>
       </c>
@@ -17385,7 +17471,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="29">
         <v>43969</v>
       </c>
@@ -17438,7 +17524,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="29">
         <v>43970</v>
       </c>
@@ -17491,7 +17577,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="29">
         <v>43971</v>
       </c>
@@ -17544,7 +17630,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="29">
         <v>43972</v>
       </c>
@@ -17597,7 +17683,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="29">
         <v>43973</v>
       </c>
@@ -17650,7 +17736,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="29">
         <v>43974</v>
       </c>
@@ -17703,7 +17789,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="29">
         <v>43975</v>
       </c>
@@ -17756,7 +17842,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="29">
         <v>43976</v>
       </c>
@@ -17809,7 +17895,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A65" s="49">
         <v>43977</v>
       </c>
@@ -17862,7 +17948,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A66" s="49">
         <v>43978</v>
       </c>
@@ -17915,7 +18001,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="49">
         <v>43979</v>
       </c>
@@ -17968,7 +18054,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="49">
         <v>43980</v>
       </c>
@@ -18021,7 +18107,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="49">
         <v>43981</v>
       </c>
@@ -18074,7 +18160,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="49">
         <v>43982</v>
       </c>
@@ -18127,7 +18213,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="49">
         <v>43983</v>
       </c>
@@ -18180,7 +18266,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" s="49">
         <v>43984</v>
       </c>
@@ -18233,7 +18319,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A73" s="49">
         <v>43985</v>
       </c>
@@ -18286,7 +18372,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" s="49">
         <v>43986</v>
       </c>
@@ -18339,7 +18425,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75" s="49">
         <v>43987</v>
       </c>
@@ -18392,7 +18478,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76" s="49">
         <v>43988</v>
       </c>
@@ -18445,7 +18531,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A77" s="49">
         <v>43989</v>
       </c>
@@ -18498,7 +18584,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A78" s="49">
         <v>43990</v>
       </c>
@@ -18551,7 +18637,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A79" s="49">
         <v>43991</v>
       </c>
@@ -18604,7 +18690,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A80" s="49">
         <v>43992</v>
       </c>
@@ -18658,7 +18744,7 @@
       </c>
       <c r="R80" s="52"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A81" s="49">
         <v>43993</v>
       </c>
@@ -18712,7 +18798,7 @@
       </c>
       <c r="R81" s="52"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A82" s="49">
         <v>43994</v>
       </c>
@@ -18766,7 +18852,7 @@
       </c>
       <c r="R82" s="52"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A83" s="49">
         <v>43995</v>
       </c>
@@ -18819,7 +18905,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A84" s="49">
         <v>43996</v>
       </c>
@@ -18872,7 +18958,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A85" s="49">
         <v>43997</v>
       </c>
@@ -18925,7 +19011,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A86" s="49">
         <v>43998</v>
       </c>
@@ -18978,7 +19064,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A87" s="49">
         <v>43999</v>
       </c>
@@ -19031,7 +19117,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A88" s="49">
         <v>44000</v>
       </c>
@@ -19084,7 +19170,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A89" s="49">
         <v>44001</v>
       </c>
@@ -19137,7 +19223,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A90" s="49">
         <v>44002</v>
       </c>
@@ -19190,7 +19276,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A91" s="49">
         <v>44003</v>
       </c>
@@ -19243,7 +19329,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A92" s="49">
         <v>44004</v>
       </c>
@@ -19296,7 +19382,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A93" s="49">
         <v>44005</v>
       </c>
@@ -19348,6 +19434,61 @@
       <c r="Q93" s="11">
         <v>512</v>
       </c>
+      <c r="R93" s="52"/>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A94" s="49">
+        <v>44006</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E94" s="11">
+        <v>51</v>
+      </c>
+      <c r="F94" s="11">
+        <v>3</v>
+      </c>
+      <c r="G94" s="11">
+        <v>47</v>
+      </c>
+      <c r="H94" s="11">
+        <v>226</v>
+      </c>
+      <c r="I94" s="11">
+        <v>7</v>
+      </c>
+      <c r="J94" s="11">
+        <v>31</v>
+      </c>
+      <c r="K94" s="11">
+        <v>118</v>
+      </c>
+      <c r="L94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P94" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q94" s="11">
+        <v>489</v>
+      </c>
+      <c r="R94" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19358,23 +19499,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R93"/>
+  <dimension ref="A1:R94"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K89" sqref="K89"/>
+      <selection pane="bottomRight" activeCell="P97" sqref="P97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.5546875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.5546875" style="2"/>
+    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.54296875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -19395,7 +19536,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -19416,7 +19557,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -19469,7 +19610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -19522,7 +19663,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -19575,7 +19716,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -19628,7 +19769,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -19681,7 +19822,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -19734,7 +19875,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -19787,7 +19928,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -19840,7 +19981,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -19893,7 +20034,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -19946,7 +20087,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -19999,7 +20140,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -20052,7 +20193,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -20105,7 +20246,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -20158,7 +20299,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -20211,7 +20352,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -20264,7 +20405,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -20317,7 +20458,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -20370,7 +20511,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -20423,7 +20564,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -20476,7 +20617,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -20529,7 +20670,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -20582,7 +20723,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -20635,7 +20776,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -20688,7 +20829,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -20741,7 +20882,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -20794,7 +20935,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -20847,7 +20988,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -20900,7 +21041,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -20953,7 +21094,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -21006,7 +21147,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -21059,7 +21200,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -21112,7 +21253,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -21165,7 +21306,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="29">
         <v>43948</v>
       </c>
@@ -21218,7 +21359,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="29">
         <v>43949</v>
       </c>
@@ -21271,7 +21412,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="29">
         <v>43950</v>
       </c>
@@ -21324,7 +21465,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="29">
         <v>43951</v>
       </c>
@@ -21377,7 +21518,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="29">
         <v>43952</v>
       </c>
@@ -21430,7 +21571,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="29">
         <v>43953</v>
       </c>
@@ -21483,7 +21624,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="29">
         <v>43954</v>
       </c>
@@ -21536,7 +21677,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="29">
         <v>43955</v>
       </c>
@@ -21589,7 +21730,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="29">
         <v>43956</v>
       </c>
@@ -21642,7 +21783,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="29">
         <v>43957</v>
       </c>
@@ -21695,7 +21836,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="29">
         <v>43958</v>
       </c>
@@ -21748,7 +21889,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="29">
         <v>43959</v>
       </c>
@@ -21801,7 +21942,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="29">
         <v>43960</v>
       </c>
@@ -21854,7 +21995,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="29">
         <v>43961</v>
       </c>
@@ -21907,7 +22048,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="29">
         <v>43962</v>
       </c>
@@ -21960,7 +22101,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="29">
         <v>43963</v>
       </c>
@@ -22013,7 +22154,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="29">
         <v>43964</v>
       </c>
@@ -22066,7 +22207,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="29">
         <v>43965</v>
       </c>
@@ -22119,7 +22260,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="29">
         <v>43966</v>
       </c>
@@ -22172,7 +22313,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="29">
         <v>43967</v>
       </c>
@@ -22225,7 +22366,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="29">
         <v>43968</v>
       </c>
@@ -22278,7 +22419,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="29">
         <v>43969</v>
       </c>
@@ -22331,7 +22472,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="29">
         <v>43970</v>
       </c>
@@ -22384,7 +22525,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="29">
         <v>43971</v>
       </c>
@@ -22437,7 +22578,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="29">
         <v>43972</v>
       </c>
@@ -22490,7 +22631,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="29">
         <v>43973</v>
       </c>
@@ -22543,7 +22684,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="29">
         <v>43974</v>
       </c>
@@ -22596,7 +22737,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="29">
         <v>43975</v>
       </c>
@@ -22649,7 +22790,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="29">
         <v>43976</v>
       </c>
@@ -22702,7 +22843,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="29">
         <v>43977</v>
       </c>
@@ -22755,7 +22896,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="29">
         <v>43978</v>
       </c>
@@ -22808,7 +22949,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="29">
         <v>43979</v>
       </c>
@@ -22861,7 +23002,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="29">
         <v>43980</v>
       </c>
@@ -22914,7 +23055,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="29">
         <v>43981</v>
       </c>
@@ -22967,7 +23108,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="29">
         <v>43982</v>
       </c>
@@ -23020,7 +23161,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="29">
         <v>43983</v>
       </c>
@@ -23073,7 +23214,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="29">
         <v>43984</v>
       </c>
@@ -23126,7 +23267,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="29">
         <v>43985</v>
       </c>
@@ -23179,7 +23320,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="29">
         <v>43986</v>
       </c>
@@ -23232,7 +23373,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="29">
         <v>43987</v>
       </c>
@@ -23285,7 +23426,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="29">
         <v>43988</v>
       </c>
@@ -23338,7 +23479,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="29">
         <v>43989</v>
       </c>
@@ -23391,7 +23532,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="29">
         <v>43990</v>
       </c>
@@ -23444,7 +23585,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="29">
         <v>43991</v>
       </c>
@@ -23497,7 +23638,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="29">
         <v>43992</v>
       </c>
@@ -23550,7 +23691,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A81" s="29">
         <v>43993</v>
       </c>
@@ -23603,7 +23744,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A82" s="29">
         <v>43994</v>
       </c>
@@ -23656,7 +23797,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A83" s="29">
         <v>43995</v>
       </c>
@@ -23709,7 +23850,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A84" s="29">
         <v>43996</v>
       </c>
@@ -23762,7 +23903,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A85" s="29">
         <v>43997</v>
       </c>
@@ -23815,7 +23956,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A86" s="29">
         <v>43998</v>
       </c>
@@ -23868,7 +24009,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A87" s="29">
         <v>43999</v>
       </c>
@@ -23921,7 +24062,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A88" s="29">
         <v>44000</v>
       </c>
@@ -23974,7 +24115,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A89" s="29">
         <v>44001</v>
       </c>
@@ -24027,7 +24168,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A90" s="29">
         <v>44002</v>
       </c>
@@ -24080,7 +24221,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A91" s="29">
         <v>44003</v>
       </c>
@@ -24134,7 +24275,7 @@
       </c>
       <c r="R91" s="52"/>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A92" s="29">
         <v>44004</v>
       </c>
@@ -24187,7 +24328,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A93" s="29">
         <v>44005</v>
       </c>
@@ -24238,6 +24379,59 @@
       </c>
       <c r="Q93" s="13">
         <v>353</v>
+      </c>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A94" s="29">
+        <v>44006</v>
+      </c>
+      <c r="B94" s="11">
+        <v>22</v>
+      </c>
+      <c r="C94" s="11">
+        <v>21</v>
+      </c>
+      <c r="D94" s="11">
+        <v>13</v>
+      </c>
+      <c r="E94" s="11">
+        <v>26</v>
+      </c>
+      <c r="F94" s="11">
+        <v>19</v>
+      </c>
+      <c r="G94" s="11">
+        <v>12</v>
+      </c>
+      <c r="H94" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I94" s="11">
+        <v>32</v>
+      </c>
+      <c r="J94" s="11">
+        <v>51</v>
+      </c>
+      <c r="K94" s="11">
+        <v>188</v>
+      </c>
+      <c r="L94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N94" s="11">
+        <v>7</v>
+      </c>
+      <c r="O94" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P94" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q94" s="13">
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -24271,7 +24465,7 @@
       <value order="0"/>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-23T11:53:43Z</value>
+      <value order="0">2020-06-24T11:09:09Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -24286,13 +24480,13 @@
       <value order="0">Being Drafted</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41913469</value>
+      <value order="0">vA41938435</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">27.12</value>
+      <value order="0">27.14</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">211</value>
+      <value order="0">213</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>

<commit_message>
Data updated by GitHub Bot (2020-06-25 20:08) (#180)
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
+++ b/output/snapshot/32397168-a637-5ecb-867e-662712036aab.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u419207\Objective\Director\Cache\erdm.scotland.gov.uk 8443 uA10434\A28088333\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u207826\Objective\Objects\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5990" windowHeight="6050" tabRatio="803" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="5985" windowHeight="6045" tabRatio="803"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2151" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       Note: NHS Borders and NHS Lothian positive cases have decreased by one and four, respectively since yesterday. These results were  reallocated to negative following revised results sent by the submitting lab. </t>
   </si>
 </sst>
 </file>
@@ -1979,6 +1982,46 @@
           </a:endParaRPr>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>11. On 25/06/2020 </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>NHS Borders and NHS Lothian positive cases decreased by one and four respectively since</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> the previous day</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>. These results were reallocated to negative following revised results sent by the submitting lab. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t> </a:t>
+          </a:r>
           <a:endParaRPr lang="en-GB" sz="1100">
             <a:effectLst/>
             <a:latin typeface="+mn-lt"/>
@@ -2658,25 +2701,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="90.453125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.453125" style="2"/>
+    <col min="1" max="1" width="3" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="90.42578125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>20</v>
       </c>
@@ -2684,7 +2727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>22</v>
       </c>
@@ -2692,13 +2735,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="23"/>
     </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
         <v>26</v>
       </c>
@@ -2706,7 +2749,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="24" t="s">
         <v>27</v>
       </c>
@@ -2714,7 +2757,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="24" t="s">
         <v>36</v>
       </c>
@@ -2722,7 +2765,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
@@ -2746,16 +2789,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O81" sqref="O81"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="M81" sqref="M81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.453125" style="2"/>
+    <col min="1" max="16384" width="9.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="44" spans="1:1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="42"/>
     </row>
   </sheetData>
@@ -2769,21 +2812,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B109" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="84" zoomScaleNormal="64" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B100" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A113" sqref="A113"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" style="2" customWidth="1"/>
-    <col min="2" max="16" width="11.453125" style="11" customWidth="1"/>
-    <col min="17" max="16384" width="8.54296875" style="2"/>
+    <col min="2" max="16" width="11.42578125" style="11" customWidth="1"/>
+    <col min="17" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2803,7 +2846,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -2822,7 +2865,7 @@
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2872,7 +2915,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43897</v>
       </c>
@@ -2922,7 +2965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>43898</v>
       </c>
@@ -2972,7 +3015,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>43899</v>
       </c>
@@ -3022,7 +3065,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>43900</v>
       </c>
@@ -3072,7 +3115,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>43901</v>
       </c>
@@ -3122,7 +3165,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>43902</v>
       </c>
@@ -3172,7 +3215,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>43903</v>
       </c>
@@ -3222,7 +3265,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>43904</v>
       </c>
@@ -3272,7 +3315,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>43905</v>
       </c>
@@ -3322,7 +3365,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>43906</v>
       </c>
@@ -3372,7 +3415,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>43907</v>
       </c>
@@ -3422,7 +3465,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>43908</v>
       </c>
@@ -3472,7 +3515,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>43909</v>
       </c>
@@ -3522,7 +3565,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>43910</v>
       </c>
@@ -3572,7 +3615,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>43911</v>
       </c>
@@ -3622,7 +3665,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>43912</v>
       </c>
@@ -3672,7 +3715,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>43913</v>
       </c>
@@ -3722,7 +3765,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>43914</v>
       </c>
@@ -3772,7 +3815,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>43915</v>
       </c>
@@ -3822,7 +3865,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>43916</v>
       </c>
@@ -3872,7 +3915,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>43917</v>
       </c>
@@ -3922,7 +3965,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>43918</v>
       </c>
@@ -3972,7 +4015,7 @@
         <v>1264</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>43919</v>
       </c>
@@ -4022,7 +4065,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>43920</v>
       </c>
@@ -4072,7 +4115,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>43921</v>
       </c>
@@ -4122,7 +4165,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>43922</v>
       </c>
@@ -4172,7 +4215,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>43923</v>
       </c>
@@ -4222,7 +4265,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>43924</v>
       </c>
@@ -4272,7 +4315,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>43925</v>
       </c>
@@ -4322,7 +4365,7 @@
         <v>3345</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>43926</v>
       </c>
@@ -4372,7 +4415,7 @@
         <v>3706</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>43927</v>
       </c>
@@ -4422,7 +4465,7 @@
         <v>3961</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>43928</v>
       </c>
@@ -4472,7 +4515,7 @@
         <v>4229</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>43929</v>
       </c>
@@ -4522,7 +4565,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>43930</v>
       </c>
@@ -4572,7 +4615,7 @@
         <v>4957</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>43931</v>
       </c>
@@ -4622,7 +4665,7 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>43932</v>
       </c>
@@ -4672,7 +4715,7 @@
         <v>5590</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>43933</v>
       </c>
@@ -4722,7 +4765,7 @@
         <v>5912</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>43934</v>
       </c>
@@ -4772,7 +4815,7 @@
         <v>6067</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>43935</v>
       </c>
@@ -4822,7 +4865,7 @@
         <v>6358</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>43936</v>
       </c>
@@ -4872,7 +4915,7 @@
         <v>6748</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43937</v>
       </c>
@@ -4922,7 +4965,7 @@
         <v>7102</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>43938</v>
       </c>
@@ -4972,7 +5015,7 @@
         <v>7409</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>43939</v>
       </c>
@@ -5022,7 +5065,7 @@
         <v>7820</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>43940</v>
       </c>
@@ -5072,7 +5115,7 @@
         <v>8187</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>43941</v>
       </c>
@@ -5122,7 +5165,7 @@
         <v>8450</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>43942</v>
       </c>
@@ -5172,7 +5215,7 @@
         <v>8672</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>43943</v>
       </c>
@@ -5222,7 +5265,7 @@
         <v>9038</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
         <v>43944</v>
       </c>
@@ -5272,7 +5315,7 @@
         <v>9409</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>43945</v>
       </c>
@@ -5322,7 +5365,7 @@
         <v>9697</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>43946</v>
       </c>
@@ -5372,7 +5415,7 @@
         <v>10051</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>43947</v>
       </c>
@@ -5423,7 +5466,7 @@
       </c>
       <c r="R54" s="37"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>43948</v>
       </c>
@@ -5474,7 +5517,7 @@
       </c>
       <c r="R55" s="37"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>43949</v>
       </c>
@@ -5525,7 +5568,7 @@
       </c>
       <c r="R56" s="38"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>43950</v>
       </c>
@@ -5575,7 +5618,7 @@
         <v>11034</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
         <v>43951</v>
       </c>
@@ -5626,7 +5669,7 @@
       </c>
       <c r="R58" s="37"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
         <v>43952</v>
       </c>
@@ -5678,7 +5721,7 @@
       <c r="R59" s="37"/>
       <c r="S59" s="37"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
         <v>43953</v>
       </c>
@@ -5728,7 +5771,7 @@
         <v>11927</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>43954</v>
       </c>
@@ -5778,7 +5821,7 @@
         <v>12097</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
         <v>43955</v>
       </c>
@@ -5828,7 +5871,7 @@
         <v>12266</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
         <v>43956</v>
       </c>
@@ -5878,7 +5921,7 @@
         <v>12437</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>43957</v>
       </c>
@@ -5928,7 +5971,7 @@
         <v>12709</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>43958</v>
       </c>
@@ -5978,7 +6021,7 @@
         <v>12924</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>43959</v>
       </c>
@@ -6028,7 +6071,7 @@
         <v>13149</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>43960</v>
       </c>
@@ -6078,7 +6121,7 @@
         <v>13305</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
         <v>43961</v>
       </c>
@@ -6128,7 +6171,7 @@
         <v>13486</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>43962</v>
       </c>
@@ -6178,7 +6221,7 @@
         <v>13627</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>43963</v>
       </c>
@@ -6228,7 +6271,7 @@
         <v>13763</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>43964</v>
       </c>
@@ -6278,7 +6321,7 @@
         <v>13929</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
         <v>43965</v>
       </c>
@@ -6328,7 +6371,7 @@
         <v>14117</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>43966</v>
       </c>
@@ -6378,7 +6421,7 @@
         <v>14260</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>43967</v>
       </c>
@@ -6428,7 +6471,7 @@
         <v>14447</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>43968</v>
       </c>
@@ -6478,7 +6521,7 @@
         <v>14537</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
         <v>43969</v>
       </c>
@@ -6528,7 +6571,7 @@
         <v>14594</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
         <v>43970</v>
       </c>
@@ -6578,7 +6621,7 @@
         <v>14655</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
         <v>43971</v>
       </c>
@@ -6628,7 +6671,7 @@
         <v>14751</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>43972</v>
       </c>
@@ -6678,7 +6721,7 @@
         <v>14856</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>43973</v>
       </c>
@@ -6728,7 +6771,7 @@
         <v>14969</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
         <v>43974</v>
       </c>
@@ -6778,7 +6821,7 @@
         <v>15041</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
         <v>43975</v>
       </c>
@@ -6828,7 +6871,7 @@
         <v>15101</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>43976</v>
       </c>
@@ -6878,7 +6921,7 @@
         <v>15156</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>43977</v>
       </c>
@@ -6928,7 +6971,7 @@
         <v>15185</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>43978</v>
       </c>
@@ -6978,7 +7021,7 @@
         <v>15240</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>43979</v>
       </c>
@@ -7028,7 +7071,7 @@
         <v>15288</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
         <v>43980</v>
       </c>
@@ -7078,7 +7121,7 @@
         <v>15327</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>43981</v>
       </c>
@@ -7128,7 +7171,7 @@
         <v>15382</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>43982</v>
       </c>
@@ -7178,7 +7221,7 @@
         <v>15400</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
         <v>43983</v>
       </c>
@@ -7228,7 +7271,7 @@
         <v>15418</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
         <v>43984</v>
       </c>
@@ -7278,7 +7321,7 @@
         <v>15471</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>43985</v>
       </c>
@@ -7328,7 +7371,7 @@
         <v>15504</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>43986</v>
       </c>
@@ -7378,7 +7421,7 @@
         <v>15553</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>43987</v>
       </c>
@@ -7428,7 +7471,7 @@
         <v>15582</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>43988</v>
       </c>
@@ -7478,7 +7521,7 @@
         <v>15603</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>43989</v>
       </c>
@@ -7528,7 +7571,7 @@
         <v>15621</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>43990</v>
       </c>
@@ -7578,7 +7621,7 @@
         <v>15639</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>43991</v>
       </c>
@@ -7628,7 +7671,7 @@
         <v>15653</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>43992</v>
       </c>
@@ -7678,7 +7721,7 @@
         <v>15665</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>43993</v>
       </c>
@@ -7728,7 +7771,7 @@
         <v>15682</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="5">
         <v>43994</v>
       </c>
@@ -7778,7 +7821,7 @@
         <v>15709</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="5">
         <v>43995</v>
       </c>
@@ -7828,7 +7871,7 @@
         <v>15730</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="53">
         <v>43996</v>
       </c>
@@ -7878,7 +7921,7 @@
         <v>15755</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:16" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>43997</v>
       </c>
@@ -7928,7 +7971,7 @@
         <v>18030</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>43998</v>
       </c>
@@ -7978,7 +8021,7 @@
         <v>18045</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>43999</v>
       </c>
@@ -8028,7 +8071,7 @@
         <v>18066</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="5">
         <v>44000</v>
       </c>
@@ -8078,7 +8121,7 @@
         <v>18077</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>44001</v>
       </c>
@@ -8128,7 +8171,7 @@
         <v>18104</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>44002</v>
       </c>
@@ -8178,7 +8221,7 @@
         <v>18130</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>44003</v>
       </c>
@@ -8228,7 +8271,7 @@
         <v>18156</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>44004</v>
       </c>
@@ -8278,7 +8321,7 @@
         <v>18170</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="5">
         <v>44005</v>
       </c>
@@ -8328,7 +8371,7 @@
         <v>18182</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="5">
         <v>44006</v>
       </c>
@@ -8378,24 +8421,60 @@
         <v>18191</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B114" s="27"/>
-      <c r="C114" s="27"/>
-      <c r="D114" s="27"/>
-      <c r="E114" s="27"/>
-      <c r="F114" s="27"/>
-      <c r="G114" s="27"/>
-      <c r="H114" s="27"/>
-      <c r="I114" s="27"/>
-      <c r="J114" s="27"/>
-      <c r="K114" s="27"/>
-      <c r="L114" s="27"/>
-      <c r="M114" s="27"/>
-      <c r="N114" s="27"/>
-      <c r="O114" s="27"/>
-      <c r="P114" s="27"/>
-    </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A114" s="5">
+        <v>44007</v>
+      </c>
+      <c r="B114" s="27">
+        <v>1252</v>
+      </c>
+      <c r="C114" s="27">
+        <v>345</v>
+      </c>
+      <c r="D114" s="27">
+        <v>285</v>
+      </c>
+      <c r="E114" s="27">
+        <v>930</v>
+      </c>
+      <c r="F114" s="27">
+        <v>1061</v>
+      </c>
+      <c r="G114" s="27">
+        <v>1414</v>
+      </c>
+      <c r="H114" s="27">
+        <v>4838</v>
+      </c>
+      <c r="I114" s="27">
+        <v>374</v>
+      </c>
+      <c r="J114" s="27">
+        <v>2716</v>
+      </c>
+      <c r="K114" s="27">
+        <v>3146</v>
+      </c>
+      <c r="L114" s="27">
+        <v>9</v>
+      </c>
+      <c r="M114" s="27">
+        <v>54</v>
+      </c>
+      <c r="N114" s="27">
+        <v>1765</v>
+      </c>
+      <c r="O114" s="27">
+        <v>7</v>
+      </c>
+      <c r="P114" s="31">
+        <v>18196</v>
+      </c>
+      <c r="Q114" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B115" s="27"/>
       <c r="C115" s="27"/>
       <c r="D115" s="27"/>
@@ -8412,7 +8491,7 @@
       <c r="O115" s="27"/>
       <c r="P115" s="27"/>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B116" s="27"/>
       <c r="C116" s="27"/>
       <c r="D116" s="27"/>
@@ -8429,7 +8508,7 @@
       <c r="O116" s="27"/>
       <c r="P116" s="27"/>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B117" s="27"/>
       <c r="C117" s="27"/>
       <c r="D117" s="27"/>
@@ -8446,7 +8525,7 @@
       <c r="O117" s="27"/>
       <c r="P117" s="27"/>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B118" s="27"/>
       <c r="C118" s="27"/>
       <c r="D118" s="27"/>
@@ -8463,7 +8542,7 @@
       <c r="O118" s="27"/>
       <c r="P118" s="27"/>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B119" s="27"/>
       <c r="C119" s="27"/>
       <c r="D119" s="27"/>
@@ -8480,7 +8559,7 @@
       <c r="O119" s="27"/>
       <c r="P119" s="27"/>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B120" s="27"/>
       <c r="C120" s="27"/>
       <c r="D120" s="27"/>
@@ -8497,7 +8576,7 @@
       <c r="O120" s="27"/>
       <c r="P120" s="27"/>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B121" s="27"/>
       <c r="C121" s="27"/>
       <c r="D121" s="27"/>
@@ -8514,7 +8593,7 @@
       <c r="O121" s="27"/>
       <c r="P121" s="27"/>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B122" s="27"/>
       <c r="C122" s="27"/>
       <c r="D122" s="27"/>
@@ -8531,7 +8610,7 @@
       <c r="O122" s="27"/>
       <c r="P122" s="27"/>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B123" s="27"/>
       <c r="C123" s="27"/>
       <c r="D123" s="27"/>
@@ -8548,7 +8627,7 @@
       <c r="O123" s="27"/>
       <c r="P123" s="27"/>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B124" s="27"/>
       <c r="C124" s="27"/>
       <c r="D124" s="27"/>
@@ -8565,7 +8644,7 @@
       <c r="O124" s="27"/>
       <c r="P124" s="27"/>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B125" s="27"/>
       <c r="C125" s="27"/>
       <c r="D125" s="27"/>
@@ -8582,7 +8661,7 @@
       <c r="O125" s="27"/>
       <c r="P125" s="27"/>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B126" s="27"/>
       <c r="C126" s="27"/>
       <c r="D126" s="27"/>
@@ -8599,7 +8678,7 @@
       <c r="O126" s="27"/>
       <c r="P126" s="27"/>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B127" s="27"/>
       <c r="C127" s="27"/>
       <c r="D127" s="27"/>
@@ -8616,7 +8695,7 @@
       <c r="O127" s="27"/>
       <c r="P127" s="27"/>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B128" s="27"/>
       <c r="C128" s="27"/>
       <c r="D128" s="27"/>
@@ -8633,7 +8712,7 @@
       <c r="O128" s="27"/>
       <c r="P128" s="27"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B129" s="27"/>
       <c r="C129" s="27"/>
       <c r="D129" s="27"/>
@@ -8650,7 +8729,7 @@
       <c r="O129" s="27"/>
       <c r="P129" s="27"/>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B130" s="27"/>
       <c r="C130" s="27"/>
       <c r="D130" s="27"/>
@@ -8667,7 +8746,7 @@
       <c r="O130" s="27"/>
       <c r="P130" s="27"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B131" s="27"/>
       <c r="C131" s="27"/>
       <c r="D131" s="27"/>
@@ -8684,7 +8763,7 @@
       <c r="O131" s="27"/>
       <c r="P131" s="27"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B132" s="27"/>
       <c r="C132" s="27"/>
       <c r="D132" s="27"/>
@@ -8701,7 +8780,7 @@
       <c r="O132" s="27"/>
       <c r="P132" s="27"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B133" s="27"/>
       <c r="C133" s="27"/>
       <c r="D133" s="27"/>
@@ -8718,7 +8797,7 @@
       <c r="O133" s="27"/>
       <c r="P133" s="27"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B134" s="27"/>
       <c r="C134" s="27"/>
       <c r="D134" s="27"/>
@@ -8735,7 +8814,7 @@
       <c r="O134" s="27"/>
       <c r="P134" s="27"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B135" s="27"/>
       <c r="C135" s="27"/>
       <c r="D135" s="27"/>
@@ -8752,7 +8831,7 @@
       <c r="O135" s="27"/>
       <c r="P135" s="27"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B136" s="27"/>
       <c r="C136" s="27"/>
       <c r="D136" s="27"/>
@@ -8769,7 +8848,7 @@
       <c r="O136" s="27"/>
       <c r="P136" s="27"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B137" s="27"/>
       <c r="C137" s="27"/>
       <c r="D137" s="27"/>
@@ -8786,7 +8865,7 @@
       <c r="O137" s="27"/>
       <c r="P137" s="27"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B138" s="27"/>
       <c r="C138" s="27"/>
       <c r="D138" s="27"/>
@@ -8803,7 +8882,7 @@
       <c r="O138" s="27"/>
       <c r="P138" s="27"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B139" s="27"/>
       <c r="C139" s="27"/>
       <c r="D139" s="27"/>
@@ -8820,7 +8899,7 @@
       <c r="O139" s="27"/>
       <c r="P139" s="27"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B140" s="27"/>
       <c r="C140" s="27"/>
       <c r="D140" s="27"/>
@@ -8837,7 +8916,7 @@
       <c r="O140" s="27"/>
       <c r="P140" s="27"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B141" s="27"/>
       <c r="C141" s="27"/>
       <c r="D141" s="27"/>
@@ -8854,7 +8933,7 @@
       <c r="O141" s="27"/>
       <c r="P141" s="27"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B142" s="27"/>
       <c r="C142" s="27"/>
       <c r="D142" s="27"/>
@@ -8871,7 +8950,7 @@
       <c r="O142" s="27"/>
       <c r="P142" s="27"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B143" s="27"/>
       <c r="C143" s="27"/>
       <c r="D143" s="27"/>
@@ -8888,7 +8967,7 @@
       <c r="O143" s="27"/>
       <c r="P143" s="27"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B144" s="27"/>
       <c r="C144" s="27"/>
       <c r="D144" s="27"/>
@@ -8905,7 +8984,7 @@
       <c r="O144" s="27"/>
       <c r="P144" s="27"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B145" s="27"/>
       <c r="C145" s="27"/>
       <c r="D145" s="27"/>
@@ -8922,7 +9001,7 @@
       <c r="O145" s="27"/>
       <c r="P145" s="27"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B146" s="27"/>
       <c r="C146" s="27"/>
       <c r="D146" s="27"/>
@@ -8939,7 +9018,7 @@
       <c r="O146" s="27"/>
       <c r="P146" s="27"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B147" s="27"/>
       <c r="C147" s="27"/>
       <c r="D147" s="27"/>
@@ -8956,7 +9035,7 @@
       <c r="O147" s="27"/>
       <c r="P147" s="27"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B148" s="27"/>
       <c r="C148" s="27"/>
       <c r="D148" s="27"/>
@@ -8973,7 +9052,7 @@
       <c r="O148" s="27"/>
       <c r="P148" s="27"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B149" s="27"/>
       <c r="C149" s="27"/>
       <c r="D149" s="27"/>
@@ -8990,7 +9069,7 @@
       <c r="O149" s="27"/>
       <c r="P149" s="27"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B150" s="27"/>
       <c r="C150" s="27"/>
       <c r="D150" s="27"/>
@@ -9007,7 +9086,7 @@
       <c r="O150" s="27"/>
       <c r="P150" s="27"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B151" s="27"/>
       <c r="C151" s="27"/>
       <c r="D151" s="27"/>
@@ -9024,7 +9103,7 @@
       <c r="O151" s="27"/>
       <c r="P151" s="27"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B152" s="27"/>
       <c r="C152" s="27"/>
       <c r="D152" s="27"/>
@@ -9041,7 +9120,7 @@
       <c r="O152" s="27"/>
       <c r="P152" s="27"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B153" s="27"/>
       <c r="C153" s="27"/>
       <c r="D153" s="27"/>
@@ -9058,7 +9137,7 @@
       <c r="O153" s="27"/>
       <c r="P153" s="27"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B154" s="27"/>
       <c r="C154" s="27"/>
       <c r="D154" s="27"/>
@@ -9075,7 +9154,7 @@
       <c r="O154" s="27"/>
       <c r="P154" s="27"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B155" s="27"/>
       <c r="C155" s="27"/>
       <c r="D155" s="27"/>
@@ -9092,7 +9171,7 @@
       <c r="O155" s="27"/>
       <c r="P155" s="27"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B156" s="27"/>
       <c r="C156" s="27"/>
       <c r="D156" s="27"/>
@@ -9109,7 +9188,7 @@
       <c r="O156" s="27"/>
       <c r="P156" s="27"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B157" s="27"/>
       <c r="C157" s="27"/>
       <c r="D157" s="27"/>
@@ -9126,7 +9205,7 @@
       <c r="O157" s="27"/>
       <c r="P157" s="27"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B158" s="27"/>
       <c r="C158" s="27"/>
       <c r="D158" s="27"/>
@@ -9143,7 +9222,7 @@
       <c r="O158" s="27"/>
       <c r="P158" s="27"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B159" s="27"/>
       <c r="C159" s="27"/>
       <c r="D159" s="27"/>
@@ -9160,7 +9239,7 @@
       <c r="O159" s="27"/>
       <c r="P159" s="27"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B160" s="27"/>
       <c r="C160" s="27"/>
       <c r="D160" s="27"/>
@@ -9186,21 +9265,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q102"/>
+  <dimension ref="A1:Q103"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q103" sqref="Q103"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.54296875" style="2"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>18</v>
       </c>
@@ -9221,7 +9300,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -9242,7 +9321,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -9295,7 +9374,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43908</v>
       </c>
@@ -9348,7 +9427,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43909</v>
       </c>
@@ -9401,7 +9480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43910</v>
       </c>
@@ -9454,7 +9533,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43911</v>
       </c>
@@ -9507,7 +9586,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43912</v>
       </c>
@@ -9560,7 +9639,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43913</v>
       </c>
@@ -9613,7 +9692,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43914</v>
       </c>
@@ -9666,7 +9745,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43915</v>
       </c>
@@ -9719,7 +9798,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43916</v>
       </c>
@@ -9772,7 +9851,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43917</v>
       </c>
@@ -9825,7 +9904,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43918</v>
       </c>
@@ -9878,7 +9957,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43919</v>
       </c>
@@ -9931,7 +10010,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43920</v>
       </c>
@@ -9984,7 +10063,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43921</v>
       </c>
@@ -10037,7 +10116,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43922</v>
       </c>
@@ -10090,7 +10169,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43923</v>
       </c>
@@ -10143,7 +10222,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43924</v>
       </c>
@@ -10196,7 +10275,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43925</v>
       </c>
@@ -10249,7 +10328,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43926</v>
       </c>
@@ -10302,7 +10381,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43927</v>
       </c>
@@ -10355,7 +10434,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43928</v>
       </c>
@@ -10408,7 +10487,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43929</v>
       </c>
@@ -10461,7 +10540,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43930</v>
       </c>
@@ -10514,7 +10593,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43931</v>
       </c>
@@ -10567,7 +10646,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43932</v>
       </c>
@@ -10620,7 +10699,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43933</v>
       </c>
@@ -10673,7 +10752,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43934</v>
       </c>
@@ -10726,7 +10805,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43935</v>
       </c>
@@ -10779,7 +10858,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43936</v>
       </c>
@@ -10832,7 +10911,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43937</v>
       </c>
@@ -10885,7 +10964,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43938</v>
       </c>
@@ -10938,7 +11017,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43939</v>
       </c>
@@ -10991,7 +11070,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="29">
         <v>43940</v>
       </c>
@@ -11044,7 +11123,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="29">
         <v>43941</v>
       </c>
@@ -11097,7 +11176,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="29">
         <v>43942</v>
       </c>
@@ -11150,7 +11229,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="29">
         <v>43943</v>
       </c>
@@ -11203,7 +11282,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="29">
         <v>43944</v>
       </c>
@@ -11256,7 +11335,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="29">
         <v>43945</v>
       </c>
@@ -11309,7 +11388,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="29">
         <v>43946</v>
       </c>
@@ -11362,7 +11441,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="29">
         <v>43947</v>
       </c>
@@ -11415,7 +11494,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="29">
         <v>43948</v>
       </c>
@@ -11468,7 +11547,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="29">
         <v>43949</v>
       </c>
@@ -11521,7 +11600,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="29">
         <v>43950</v>
       </c>
@@ -11574,7 +11653,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="29">
         <v>43951</v>
       </c>
@@ -11627,7 +11706,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="29">
         <v>43952</v>
       </c>
@@ -11680,7 +11759,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="29">
         <v>43953</v>
       </c>
@@ -11733,7 +11812,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="29">
         <v>43954</v>
       </c>
@@ -11786,7 +11865,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="29">
         <v>43955</v>
       </c>
@@ -11839,7 +11918,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="29">
         <v>43956</v>
       </c>
@@ -11892,7 +11971,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="29">
         <v>43957</v>
       </c>
@@ -11945,7 +12024,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="29">
         <v>43958</v>
       </c>
@@ -11998,7 +12077,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="29">
         <v>43959</v>
       </c>
@@ -12051,7 +12130,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="29">
         <v>43960</v>
       </c>
@@ -12104,7 +12183,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="29">
         <v>43961</v>
       </c>
@@ -12157,7 +12236,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="29">
         <v>43962</v>
       </c>
@@ -12210,7 +12289,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="29">
         <v>43963</v>
       </c>
@@ -12263,7 +12342,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="29">
         <v>43964</v>
       </c>
@@ -12316,7 +12395,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="29">
         <v>43965</v>
       </c>
@@ -12369,7 +12448,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="29">
         <v>43966</v>
       </c>
@@ -12422,7 +12501,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="29">
         <v>43967</v>
       </c>
@@ -12475,7 +12554,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="29">
         <v>43968</v>
       </c>
@@ -12528,7 +12607,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="29">
         <v>43969</v>
       </c>
@@ -12581,7 +12660,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="29">
         <v>43970</v>
       </c>
@@ -12634,7 +12713,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="29">
         <v>43971</v>
       </c>
@@ -12687,7 +12766,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="29">
         <v>43972</v>
       </c>
@@ -12740,7 +12819,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="29">
         <v>43973</v>
       </c>
@@ -12793,7 +12872,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="29">
         <v>43974</v>
       </c>
@@ -12846,7 +12925,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="29">
         <v>43975</v>
       </c>
@@ -12899,7 +12978,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="29">
         <v>43976</v>
       </c>
@@ -12952,7 +13031,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="29">
         <v>43977</v>
       </c>
@@ -13005,7 +13084,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="29">
         <v>43978</v>
       </c>
@@ -13058,7 +13137,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="29">
         <v>43979</v>
       </c>
@@ -13111,7 +13190,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="29">
         <v>43980</v>
       </c>
@@ -13164,7 +13243,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="29">
         <v>43981</v>
       </c>
@@ -13217,7 +13296,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="29">
         <v>43982</v>
       </c>
@@ -13270,7 +13349,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="29">
         <v>43983</v>
       </c>
@@ -13323,7 +13402,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="29">
         <v>43984</v>
       </c>
@@ -13376,7 +13455,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="29">
         <v>43985</v>
       </c>
@@ -13429,7 +13508,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" s="29">
         <v>43986</v>
       </c>
@@ -13482,7 +13561,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="29">
         <v>43987</v>
       </c>
@@ -13535,7 +13614,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" s="29">
         <v>43988</v>
       </c>
@@ -13588,7 +13667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="29">
         <v>43989</v>
       </c>
@@ -13641,7 +13720,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="29">
         <v>43990</v>
       </c>
@@ -13694,7 +13773,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="29">
         <v>43991</v>
       </c>
@@ -13747,7 +13826,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" s="29">
         <v>43992</v>
       </c>
@@ -13800,7 +13879,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="29">
         <v>43993</v>
       </c>
@@ -13853,7 +13932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="29">
         <v>43994</v>
       </c>
@@ -13906,7 +13985,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="29">
         <v>43995</v>
       </c>
@@ -13959,7 +14038,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="29">
         <v>43996</v>
       </c>
@@ -14012,7 +14091,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="29">
         <v>43997</v>
       </c>
@@ -14065,7 +14144,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="29">
         <v>43998</v>
       </c>
@@ -14118,7 +14197,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="29">
         <v>43999</v>
       </c>
@@ -14171,7 +14250,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="29">
         <v>44000</v>
       </c>
@@ -14224,7 +14303,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="29">
         <v>44001</v>
       </c>
@@ -14277,7 +14356,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" s="29">
         <v>44002</v>
       </c>
@@ -14330,7 +14409,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="29">
         <v>44003</v>
       </c>
@@ -14383,7 +14462,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" s="29">
         <v>44004</v>
       </c>
@@ -14436,7 +14515,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="29">
         <v>44005</v>
       </c>
@@ -14489,7 +14568,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="29">
         <v>44006</v>
       </c>
@@ -14540,6 +14619,59 @@
       </c>
       <c r="Q102" s="13">
         <v>23</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C103" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D103" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E103" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F103" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G103" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H103" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I103" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J103" s="11">
+        <v>5</v>
+      </c>
+      <c r="K103" s="11">
+        <v>5</v>
+      </c>
+      <c r="L103" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M103" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N103" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O103" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P103" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q103" s="13">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -14551,23 +14683,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R94"/>
+  <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P90" sqref="P90"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.54296875" style="2"/>
+    <col min="1" max="1" width="15.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -14588,7 +14720,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -14609,7 +14741,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -14662,7 +14794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -14715,7 +14847,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -14768,7 +14900,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -14821,7 +14953,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -14874,7 +15006,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -14927,7 +15059,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -14980,7 +15112,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -15033,7 +15165,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -15086,7 +15218,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -15139,7 +15271,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -15192,7 +15324,7 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -15245,7 +15377,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -15298,7 +15430,7 @@
         <v>1262</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -15351,7 +15483,7 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -15404,7 +15536,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -15457,7 +15589,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -15510,7 +15642,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -15563,7 +15695,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -15616,7 +15748,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -15669,7 +15801,7 @@
         <v>1482</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -15722,7 +15854,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -15775,7 +15907,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -15828,7 +15960,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -15881,7 +16013,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -15934,7 +16066,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -15987,7 +16119,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -16040,7 +16172,7 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -16093,7 +16225,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -16146,7 +16278,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -16199,7 +16331,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -16252,7 +16384,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -16305,7 +16437,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -16358,7 +16490,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="29">
         <v>43948</v>
       </c>
@@ -16411,7 +16543,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="29">
         <v>43949</v>
       </c>
@@ -16464,7 +16596,7 @@
         <v>1359</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="29">
         <v>43950</v>
       </c>
@@ -16517,7 +16649,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="29">
         <v>43951</v>
       </c>
@@ -16570,7 +16702,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="29">
         <v>43952</v>
       </c>
@@ -16623,7 +16755,7 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="29">
         <v>43953</v>
       </c>
@@ -16676,7 +16808,7 @@
         <v>1277</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="29">
         <v>43954</v>
       </c>
@@ -16729,7 +16861,7 @@
         <v>1266</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="29">
         <v>43955</v>
       </c>
@@ -16782,7 +16914,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="29">
         <v>43956</v>
       </c>
@@ -16835,7 +16967,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="29">
         <v>43957</v>
       </c>
@@ -16888,7 +17020,7 @@
         <v>1204</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="29">
         <v>43958</v>
       </c>
@@ -16941,7 +17073,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="29">
         <v>43959</v>
       </c>
@@ -16994,7 +17126,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="29">
         <v>43960</v>
       </c>
@@ -17047,7 +17179,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="29">
         <v>43961</v>
       </c>
@@ -17100,7 +17232,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="29">
         <v>43962</v>
       </c>
@@ -17153,7 +17285,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="29">
         <v>43963</v>
       </c>
@@ -17206,7 +17338,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="29">
         <v>43964</v>
       </c>
@@ -17259,7 +17391,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="29">
         <v>43965</v>
       </c>
@@ -17312,7 +17444,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="29">
         <v>43966</v>
       </c>
@@ -17365,7 +17497,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="29">
         <v>43967</v>
       </c>
@@ -17418,7 +17550,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="29">
         <v>43968</v>
       </c>
@@ -17471,7 +17603,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="29">
         <v>43969</v>
       </c>
@@ -17524,7 +17656,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="29">
         <v>43970</v>
       </c>
@@ -17577,7 +17709,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="29">
         <v>43971</v>
       </c>
@@ -17630,7 +17762,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="29">
         <v>43972</v>
       </c>
@@ -17683,7 +17815,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="29">
         <v>43973</v>
       </c>
@@ -17736,7 +17868,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="29">
         <v>43974</v>
       </c>
@@ -17789,7 +17921,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="29">
         <v>43975</v>
       </c>
@@ -17842,7 +17974,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="29">
         <v>43976</v>
       </c>
@@ -17895,7 +18027,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="49">
         <v>43977</v>
       </c>
@@ -17948,7 +18080,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="49">
         <v>43978</v>
       </c>
@@ -18001,7 +18133,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="49">
         <v>43979</v>
       </c>
@@ -18054,7 +18186,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="49">
         <v>43980</v>
       </c>
@@ -18107,7 +18239,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="49">
         <v>43981</v>
       </c>
@@ -18160,7 +18292,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="49">
         <v>43982</v>
       </c>
@@ -18213,7 +18345,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="49">
         <v>43983</v>
       </c>
@@ -18266,7 +18398,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="49">
         <v>43984</v>
       </c>
@@ -18319,7 +18451,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="49">
         <v>43985</v>
       </c>
@@ -18372,7 +18504,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="49">
         <v>43986</v>
       </c>
@@ -18425,7 +18557,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="49">
         <v>43987</v>
       </c>
@@ -18478,7 +18610,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="49">
         <v>43988</v>
       </c>
@@ -18531,7 +18663,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="49">
         <v>43989</v>
       </c>
@@ -18584,7 +18716,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="49">
         <v>43990</v>
       </c>
@@ -18637,7 +18769,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="49">
         <v>43991</v>
       </c>
@@ -18690,7 +18822,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="49">
         <v>43992</v>
       </c>
@@ -18744,7 +18876,7 @@
       </c>
       <c r="R80" s="52"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="49">
         <v>43993</v>
       </c>
@@ -18798,7 +18930,7 @@
       </c>
       <c r="R81" s="52"/>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="49">
         <v>43994</v>
       </c>
@@ -18852,7 +18984,7 @@
       </c>
       <c r="R82" s="52"/>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="49">
         <v>43995</v>
       </c>
@@ -18905,7 +19037,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="49">
         <v>43996</v>
       </c>
@@ -18958,7 +19090,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="49">
         <v>43997</v>
       </c>
@@ -19011,7 +19143,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="49">
         <v>43998</v>
       </c>
@@ -19064,7 +19196,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="49">
         <v>43999</v>
       </c>
@@ -19117,7 +19249,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="49">
         <v>44000</v>
       </c>
@@ -19170,7 +19302,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="49">
         <v>44001</v>
       </c>
@@ -19223,7 +19355,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="49">
         <v>44002</v>
       </c>
@@ -19276,7 +19408,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="49">
         <v>44003</v>
       </c>
@@ -19329,7 +19461,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="49">
         <v>44004</v>
       </c>
@@ -19382,7 +19514,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="49">
         <v>44005</v>
       </c>
@@ -19436,7 +19568,7 @@
       </c>
       <c r="R93" s="52"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="49">
         <v>44006</v>
       </c>
@@ -19452,8 +19584,8 @@
       <c r="E94" s="11">
         <v>51</v>
       </c>
-      <c r="F94" s="11">
-        <v>3</v>
+      <c r="F94" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="G94" s="11">
         <v>47</v>
@@ -19489,6 +19621,59 @@
         <v>489</v>
       </c>
       <c r="R94" s="52"/>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A95" s="49">
+        <v>44007</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E95" s="11">
+        <v>49</v>
+      </c>
+      <c r="F95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G95" s="11">
+        <v>49</v>
+      </c>
+      <c r="H95" s="11">
+        <v>215</v>
+      </c>
+      <c r="I95" s="11">
+        <v>8</v>
+      </c>
+      <c r="J95" s="11">
+        <v>30</v>
+      </c>
+      <c r="K95" s="11">
+        <v>112</v>
+      </c>
+      <c r="L95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N95" s="11">
+        <v>5</v>
+      </c>
+      <c r="O95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P95" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q95" s="13">
+        <v>472</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19499,23 +19684,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R94"/>
+  <dimension ref="A1:R95"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P97" sqref="P97"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" style="11" customWidth="1"/>
-    <col min="2" max="17" width="10.54296875" style="11" customWidth="1"/>
-    <col min="18" max="16384" width="8.54296875" style="2"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="2" max="17" width="10.5703125" style="11" customWidth="1"/>
+    <col min="18" max="16384" width="8.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -19536,7 +19721,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>30</v>
       </c>
@@ -19557,7 +19742,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
@@ -19610,7 +19795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>43916</v>
       </c>
@@ -19663,7 +19848,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>43917</v>
       </c>
@@ -19716,7 +19901,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>43918</v>
       </c>
@@ -19769,7 +19954,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>43919</v>
       </c>
@@ -19822,7 +20007,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>43920</v>
       </c>
@@ -19875,7 +20060,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>43921</v>
       </c>
@@ -19928,7 +20113,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>43922</v>
       </c>
@@ -19981,7 +20166,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>43923</v>
       </c>
@@ -20034,7 +20219,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>43924</v>
       </c>
@@ -20087,7 +20272,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>43925</v>
       </c>
@@ -20140,7 +20325,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>43926</v>
       </c>
@@ -20193,7 +20378,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>43927</v>
       </c>
@@ -20246,7 +20431,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>43928</v>
       </c>
@@ -20299,7 +20484,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>43929</v>
       </c>
@@ -20352,7 +20537,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>43930</v>
       </c>
@@ -20405,7 +20590,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>43931</v>
       </c>
@@ -20458,7 +20643,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>43932</v>
       </c>
@@ -20511,7 +20696,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>43933</v>
       </c>
@@ -20564,7 +20749,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>43934</v>
       </c>
@@ -20617,7 +20802,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>43935</v>
       </c>
@@ -20670,7 +20855,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>43936</v>
       </c>
@@ -20723,7 +20908,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>43937</v>
       </c>
@@ -20776,7 +20961,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>43938</v>
       </c>
@@ -20829,7 +21014,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>43939</v>
       </c>
@@ -20882,7 +21067,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>43940</v>
       </c>
@@ -20935,7 +21120,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12">
         <v>43941</v>
       </c>
@@ -20988,7 +21173,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12">
         <v>43942</v>
       </c>
@@ -21041,7 +21226,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12">
         <v>43943</v>
       </c>
@@ -21094,7 +21279,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12">
         <v>43944</v>
       </c>
@@ -21147,7 +21332,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="12">
         <v>43945</v>
       </c>
@@ -21200,7 +21385,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12">
         <v>43946</v>
       </c>
@@ -21253,7 +21438,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="12">
         <v>43947</v>
       </c>
@@ -21306,7 +21491,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="29">
         <v>43948</v>
       </c>
@@ -21359,7 +21544,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="29">
         <v>43949</v>
       </c>
@@ -21412,7 +21597,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="29">
         <v>43950</v>
       </c>
@@ -21465,7 +21650,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="29">
         <v>43951</v>
       </c>
@@ -21518,7 +21703,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="29">
         <v>43952</v>
       </c>
@@ -21571,7 +21756,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" s="29">
         <v>43953</v>
       </c>
@@ -21624,7 +21809,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="29">
         <v>43954</v>
       </c>
@@ -21677,7 +21862,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="29">
         <v>43955</v>
       </c>
@@ -21730,7 +21915,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" s="29">
         <v>43956</v>
       </c>
@@ -21783,7 +21968,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="29">
         <v>43957</v>
       </c>
@@ -21836,7 +22021,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="29">
         <v>43958</v>
       </c>
@@ -21889,7 +22074,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="29">
         <v>43959</v>
       </c>
@@ -21942,7 +22127,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="29">
         <v>43960</v>
       </c>
@@ -21995,7 +22180,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="29">
         <v>43961</v>
       </c>
@@ -22048,7 +22233,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="29">
         <v>43962</v>
       </c>
@@ -22101,7 +22286,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="29">
         <v>43963</v>
       </c>
@@ -22154,7 +22339,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="29">
         <v>43964</v>
       </c>
@@ -22207,7 +22392,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="29">
         <v>43965</v>
       </c>
@@ -22260,7 +22445,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="29">
         <v>43966</v>
       </c>
@@ -22313,7 +22498,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="29">
         <v>43967</v>
       </c>
@@ -22366,7 +22551,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="29">
         <v>43968</v>
       </c>
@@ -22419,7 +22604,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="29">
         <v>43969</v>
       </c>
@@ -22472,7 +22657,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="29">
         <v>43970</v>
       </c>
@@ -22525,7 +22710,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="29">
         <v>43971</v>
       </c>
@@ -22578,7 +22763,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="29">
         <v>43972</v>
       </c>
@@ -22631,7 +22816,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="29">
         <v>43973</v>
       </c>
@@ -22684,7 +22869,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="29">
         <v>43974</v>
       </c>
@@ -22737,7 +22922,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="29">
         <v>43975</v>
       </c>
@@ -22790,7 +22975,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="29">
         <v>43976</v>
       </c>
@@ -22843,7 +23028,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="29">
         <v>43977</v>
       </c>
@@ -22896,7 +23081,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="29">
         <v>43978</v>
       </c>
@@ -22949,7 +23134,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="29">
         <v>43979</v>
       </c>
@@ -23002,7 +23187,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="29">
         <v>43980</v>
       </c>
@@ -23055,7 +23240,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="29">
         <v>43981</v>
       </c>
@@ -23108,7 +23293,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="29">
         <v>43982</v>
       </c>
@@ -23161,7 +23346,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="29">
         <v>43983</v>
       </c>
@@ -23214,7 +23399,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="29">
         <v>43984</v>
       </c>
@@ -23267,7 +23452,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="29">
         <v>43985</v>
       </c>
@@ -23320,7 +23505,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="29">
         <v>43986</v>
       </c>
@@ -23373,7 +23558,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="29">
         <v>43987</v>
       </c>
@@ -23426,7 +23611,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="29">
         <v>43988</v>
       </c>
@@ -23479,7 +23664,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="29">
         <v>43989</v>
       </c>
@@ -23532,7 +23717,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="29">
         <v>43990</v>
       </c>
@@ -23585,7 +23770,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="29">
         <v>43991</v>
       </c>
@@ -23638,7 +23823,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="29">
         <v>43992</v>
       </c>
@@ -23691,7 +23876,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="29">
         <v>43993</v>
       </c>
@@ -23744,7 +23929,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="29">
         <v>43994</v>
       </c>
@@ -23797,7 +23982,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="29">
         <v>43995</v>
       </c>
@@ -23850,7 +24035,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="29">
         <v>43996</v>
       </c>
@@ -23903,7 +24088,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="29">
         <v>43997</v>
       </c>
@@ -23956,7 +24141,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="29">
         <v>43998</v>
       </c>
@@ -24009,7 +24194,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="29">
         <v>43999</v>
       </c>
@@ -24062,7 +24247,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="29">
         <v>44000</v>
       </c>
@@ -24115,7 +24300,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="29">
         <v>44001</v>
       </c>
@@ -24168,7 +24353,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="29">
         <v>44002</v>
       </c>
@@ -24221,7 +24406,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="29">
         <v>44003</v>
       </c>
@@ -24275,7 +24460,7 @@
       </c>
       <c r="R91" s="52"/>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="29">
         <v>44004</v>
       </c>
@@ -24328,7 +24513,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="29">
         <v>44005</v>
       </c>
@@ -24381,7 +24566,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="29">
         <v>44006</v>
       </c>
@@ -24432,6 +24617,59 @@
       </c>
       <c r="Q94" s="13">
         <v>391</v>
+      </c>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A95" s="29">
+        <v>44007</v>
+      </c>
+      <c r="B95" s="11">
+        <v>23</v>
+      </c>
+      <c r="C95" s="11">
+        <v>15</v>
+      </c>
+      <c r="D95" s="11">
+        <v>10</v>
+      </c>
+      <c r="E95" s="11">
+        <v>14</v>
+      </c>
+      <c r="F95" s="11">
+        <v>24</v>
+      </c>
+      <c r="G95" s="11">
+        <v>14</v>
+      </c>
+      <c r="H95" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I95" s="11">
+        <v>27</v>
+      </c>
+      <c r="J95" s="11">
+        <v>66</v>
+      </c>
+      <c r="K95" s="11">
+        <v>151</v>
+      </c>
+      <c r="L95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="N95" s="11">
+        <v>9</v>
+      </c>
+      <c r="O95" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P95" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q95" s="13">
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -24459,13 +24697,13 @@
       <value order="0">false</value>
     </field>
     <field name="Objective-IsPublished">
-      <value order="0">false</value>
+      <value order="0">true</value>
     </field>
     <field name="Objective-DatePublished">
-      <value order="0"/>
+      <value order="0">2020-06-25T16:28:26Z</value>
     </field>
     <field name="Objective-ModificationStamp">
-      <value order="0">2020-06-24T11:09:09Z</value>
+      <value order="0">2020-06-25T16:28:27Z</value>
     </field>
     <field name="Objective-Owner">
       <value order="0">Grant, Neil N (u207826)</value>
@@ -24477,16 +24715,16 @@
       <value order="0">Analytical: COVID 19 Analysis: Restricted working papers: Research and analysis: Diseases: 2020-2025</value>
     </field>
     <field name="Objective-State">
-      <value order="0">Being Drafted</value>
+      <value order="0">Published</value>
     </field>
     <field name="Objective-VersionId">
-      <value order="0">vA41938435</value>
+      <value order="0">vA41974355</value>
     </field>
     <field name="Objective-Version">
-      <value order="0">27.14</value>
+      <value order="0">29.0</value>
     </field>
     <field name="Objective-VersionNumber">
-      <value order="0">213</value>
+      <value order="0">219</value>
     </field>
     <field name="Objective-VersionComment">
       <value order="0"/>

</xml_diff>